<commit_message>
I think I made it all!
</commit_message>
<xml_diff>
--- a/src/processed.xlsx
+++ b/src/processed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\문서\My Projects\202406\imsorry\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212257E4-F7DC-4A7C-86CF-2CDC53E64DEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90823E44-2A44-4DB6-AD1A-8991F152E3DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8830,13 +8830,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AD527"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L526" sqref="L526"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="S216" sqref="S216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -8929,7 +8929,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:30" ht="12.75" hidden="1">
+    <row r="2" spans="1:30" ht="12.75">
       <c r="A2" s="4">
         <v>61381154966</v>
       </c>
@@ -9011,7 +9011,7 @@
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
     </row>
-    <row r="3" spans="1:30" ht="12.75" hidden="1">
+    <row r="3" spans="1:30" ht="12.75">
       <c r="A3" s="4">
         <v>12381005306</v>
       </c>
@@ -9093,7 +9093,7 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:30" ht="12.75" hidden="1">
+    <row r="4" spans="1:30" ht="12.75">
       <c r="A4" s="4">
         <v>61181014156</v>
       </c>
@@ -9175,7 +9175,7 @@
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
-    <row r="5" spans="1:30" ht="12.75" hidden="1">
+    <row r="5" spans="1:30" ht="12.75">
       <c r="A5" s="4">
         <v>20781474876</v>
       </c>
@@ -9257,7 +9257,7 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
-    <row r="6" spans="1:30" ht="12.75" hidden="1">
+    <row r="6" spans="1:30" ht="12.75">
       <c r="A6" s="4">
         <v>12486557276</v>
       </c>
@@ -9337,7 +9337,7 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
     </row>
-    <row r="7" spans="1:30" ht="12.75" hidden="1">
+    <row r="7" spans="1:30" ht="12.75">
       <c r="A7" s="4">
         <v>10181349286</v>
       </c>
@@ -9417,7 +9417,7 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
     </row>
-    <row r="8" spans="1:30" ht="12.75" hidden="1">
+    <row r="8" spans="1:30" ht="12.75">
       <c r="A8" s="4">
         <v>11481588536</v>
       </c>
@@ -9497,7 +9497,7 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
-    <row r="9" spans="1:30" ht="12.75" hidden="1">
+    <row r="9" spans="1:30" ht="12.75">
       <c r="A9" s="4">
         <v>12486838786</v>
       </c>
@@ -9577,7 +9577,7 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
     </row>
-    <row r="10" spans="1:30" ht="12.75" hidden="1">
+    <row r="10" spans="1:30" ht="12.75">
       <c r="A10" s="4">
         <v>20181441586</v>
       </c>
@@ -9657,7 +9657,7 @@
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
     </row>
-    <row r="11" spans="1:30" ht="12.75" hidden="1">
+    <row r="11" spans="1:30" ht="12.75">
       <c r="A11" s="4">
         <v>40981089646</v>
       </c>
@@ -9737,7 +9737,7 @@
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
     </row>
-    <row r="12" spans="1:30" ht="12.75" hidden="1">
+    <row r="12" spans="1:30" ht="12.75">
       <c r="A12" s="4">
         <v>14081860236</v>
       </c>
@@ -9817,7 +9817,7 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
     </row>
-    <row r="13" spans="1:30" ht="12.75" hidden="1">
+    <row r="13" spans="1:30" ht="12.75">
       <c r="A13" s="4">
         <v>41081430356</v>
       </c>
@@ -9897,7 +9897,7 @@
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
     </row>
-    <row r="14" spans="1:30" ht="12.75" hidden="1">
+    <row r="14" spans="1:30" ht="12.75">
       <c r="A14" s="4">
         <v>11481588536</v>
       </c>
@@ -9977,7 +9977,7 @@
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
     </row>
-    <row r="15" spans="1:30" ht="12.75" hidden="1">
+    <row r="15" spans="1:30" ht="12.75">
       <c r="A15" s="4">
         <v>21181818826</v>
       </c>
@@ -10057,7 +10057,7 @@
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
     </row>
-    <row r="16" spans="1:30" ht="12.75" hidden="1">
+    <row r="16" spans="1:30" ht="12.75">
       <c r="A16" s="4">
         <v>22081193306</v>
       </c>
@@ -10137,7 +10137,7 @@
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
     </row>
-    <row r="17" spans="1:30" ht="12.75" hidden="1">
+    <row r="17" spans="1:30" ht="12.75">
       <c r="A17" s="4">
         <v>10981431736</v>
       </c>
@@ -10217,7 +10217,7 @@
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
     </row>
-    <row r="18" spans="1:30" ht="12.75" hidden="1">
+    <row r="18" spans="1:30" ht="12.75">
       <c r="A18" s="4">
         <v>12981589146</v>
       </c>
@@ -10297,7 +10297,7 @@
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
     </row>
-    <row r="19" spans="1:30" ht="12.75" hidden="1">
+    <row r="19" spans="1:30" ht="12.75">
       <c r="A19" s="4">
         <v>50281451766</v>
       </c>
@@ -10377,7 +10377,7 @@
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
     </row>
-    <row r="20" spans="1:30" ht="12.75" hidden="1">
+    <row r="20" spans="1:30" ht="12.75">
       <c r="A20" s="4">
         <v>60986170206</v>
       </c>
@@ -10455,7 +10455,7 @@
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
     </row>
-    <row r="21" spans="1:30" ht="12.75" hidden="1">
+    <row r="21" spans="1:30" ht="12.75">
       <c r="A21" s="4">
         <v>40281141316</v>
       </c>
@@ -10531,7 +10531,7 @@
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
     </row>
-    <row r="22" spans="1:30" ht="12.75" hidden="1">
+    <row r="22" spans="1:30" ht="12.75">
       <c r="A22" s="4">
         <v>41081430356</v>
       </c>
@@ -10611,7 +10611,7 @@
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
     </row>
-    <row r="23" spans="1:30" ht="12.75" hidden="1">
+    <row r="23" spans="1:30" ht="12.75">
       <c r="A23" s="4">
         <v>31281096556</v>
       </c>
@@ -10691,7 +10691,7 @@
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
     </row>
-    <row r="24" spans="1:30" ht="12.75" hidden="1">
+    <row r="24" spans="1:30" ht="12.75">
       <c r="A24" s="4">
         <v>10181349286</v>
       </c>
@@ -10771,7 +10771,7 @@
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
     </row>
-    <row r="25" spans="1:30" ht="12.75" hidden="1">
+    <row r="25" spans="1:30" ht="12.75">
       <c r="A25" s="4">
         <v>60481181796</v>
       </c>
@@ -10851,7 +10851,7 @@
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
     </row>
-    <row r="26" spans="1:30" ht="12.75" hidden="1">
+    <row r="26" spans="1:30" ht="12.75">
       <c r="A26" s="4">
         <v>12381560866</v>
       </c>
@@ -10931,7 +10931,7 @@
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
     </row>
-    <row r="27" spans="1:30" ht="12.75" hidden="1">
+    <row r="27" spans="1:30" ht="12.75">
       <c r="A27" s="4">
         <v>31481079546</v>
       </c>
@@ -11011,7 +11011,7 @@
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
     </row>
-    <row r="28" spans="1:30" ht="12.75" hidden="1">
+    <row r="28" spans="1:30" ht="12.75">
       <c r="A28" s="4">
         <v>41881016506</v>
       </c>
@@ -11091,7 +11091,7 @@
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
     </row>
-    <row r="29" spans="1:30" ht="12.75" hidden="1">
+    <row r="29" spans="1:30" ht="12.75">
       <c r="A29" s="4">
         <v>60481168706</v>
       </c>
@@ -11171,7 +11171,7 @@
       <c r="AC29" s="3"/>
       <c r="AD29" s="3"/>
     </row>
-    <row r="30" spans="1:30" ht="12.75" hidden="1">
+    <row r="30" spans="1:30" ht="12.75">
       <c r="A30" s="4">
         <v>41281077346</v>
       </c>
@@ -11251,7 +11251,7 @@
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
     </row>
-    <row r="31" spans="1:30" ht="12.75" hidden="1">
+    <row r="31" spans="1:30" ht="12.75">
       <c r="A31" s="4">
         <v>60981463796</v>
       </c>
@@ -11331,7 +11331,7 @@
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
     </row>
-    <row r="32" spans="1:30" ht="12.75" hidden="1">
+    <row r="32" spans="1:30" ht="12.75">
       <c r="A32" s="4">
         <v>40881684316</v>
       </c>
@@ -11411,7 +11411,7 @@
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
     </row>
-    <row r="33" spans="1:30" ht="12.75" hidden="1">
+    <row r="33" spans="1:30" ht="12.75">
       <c r="A33" s="4">
         <v>60981463796</v>
       </c>
@@ -11491,7 +11491,7 @@
       <c r="AC33" s="3"/>
       <c r="AD33" s="3"/>
     </row>
-    <row r="34" spans="1:30" ht="12.75" hidden="1">
+    <row r="34" spans="1:30" ht="12.75">
       <c r="A34" s="4">
         <v>11481004816</v>
       </c>
@@ -11571,7 +11571,7 @@
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
     </row>
-    <row r="35" spans="1:30" ht="12.75" hidden="1">
+    <row r="35" spans="1:30" ht="12.75">
       <c r="A35" s="4">
         <v>90702173657</v>
       </c>
@@ -11651,7 +11651,7 @@
       <c r="AC35" s="3"/>
       <c r="AD35" s="3"/>
     </row>
-    <row r="36" spans="1:30" ht="12.75" hidden="1">
+    <row r="36" spans="1:30" ht="12.75">
       <c r="A36" s="4">
         <v>50681022806</v>
       </c>
@@ -11731,7 +11731,7 @@
       <c r="AC36" s="3"/>
       <c r="AD36" s="3"/>
     </row>
-    <row r="37" spans="1:30" ht="12.75" hidden="1">
+    <row r="37" spans="1:30" ht="12.75">
       <c r="A37" s="4">
         <v>60781542336</v>
       </c>
@@ -11811,7 +11811,7 @@
       <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
     </row>
-    <row r="38" spans="1:30" ht="12.75" hidden="1">
+    <row r="38" spans="1:30" ht="12.75">
       <c r="A38" s="4">
         <v>10281317546</v>
       </c>
@@ -11891,7 +11891,7 @@
       <c r="AC38" s="3"/>
       <c r="AD38" s="3"/>
     </row>
-    <row r="39" spans="1:30" ht="12.75" hidden="1">
+    <row r="39" spans="1:30" ht="12.75">
       <c r="A39" s="4">
         <v>22081040506</v>
       </c>
@@ -11971,7 +11971,7 @@
       <c r="AC39" s="3"/>
       <c r="AD39" s="3"/>
     </row>
-    <row r="40" spans="1:30" ht="12.75" hidden="1">
+    <row r="40" spans="1:30" ht="12.75">
       <c r="A40" s="4">
         <v>22081193306</v>
       </c>
@@ -12051,7 +12051,7 @@
       <c r="AC40" s="3"/>
       <c r="AD40" s="3"/>
     </row>
-    <row r="41" spans="1:30" ht="12.75" hidden="1">
+    <row r="41" spans="1:30" ht="12.75">
       <c r="A41" s="4">
         <v>11281209006</v>
       </c>
@@ -12131,7 +12131,7 @@
       <c r="AC41" s="3"/>
       <c r="AD41" s="3"/>
     </row>
-    <row r="42" spans="1:30" ht="12.75" hidden="1">
+    <row r="42" spans="1:30" ht="12.75">
       <c r="A42" s="4">
         <v>90700104187</v>
       </c>
@@ -12211,7 +12211,7 @@
       <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
     </row>
-    <row r="43" spans="1:30" ht="12.75" hidden="1">
+    <row r="43" spans="1:30" ht="12.75">
       <c r="A43" s="4">
         <v>61781336146</v>
       </c>
@@ -12291,7 +12291,7 @@
       <c r="AC43" s="3"/>
       <c r="AD43" s="3"/>
     </row>
-    <row r="44" spans="1:30" ht="12.75" hidden="1">
+    <row r="44" spans="1:30" ht="12.75">
       <c r="A44" s="4">
         <v>11481482586</v>
       </c>
@@ -12371,7 +12371,7 @@
       <c r="AC44" s="3"/>
       <c r="AD44" s="3"/>
     </row>
-    <row r="45" spans="1:30" ht="12.75" hidden="1">
+    <row r="45" spans="1:30" ht="12.75">
       <c r="A45" s="4">
         <v>11481482586</v>
       </c>
@@ -12451,7 +12451,7 @@
       <c r="AC45" s="3"/>
       <c r="AD45" s="3"/>
     </row>
-    <row r="46" spans="1:30" ht="12.75" hidden="1">
+    <row r="46" spans="1:30" ht="12.75">
       <c r="A46" s="4">
         <v>50681022806</v>
       </c>
@@ -12531,7 +12531,7 @@
       <c r="AC46" s="3"/>
       <c r="AD46" s="3"/>
     </row>
-    <row r="47" spans="1:30" ht="12.75" hidden="1">
+    <row r="47" spans="1:30" ht="12.75">
       <c r="A47" s="4">
         <v>13981126716</v>
       </c>
@@ -12611,7 +12611,7 @@
       <c r="AC47" s="3"/>
       <c r="AD47" s="3"/>
     </row>
-    <row r="48" spans="1:30" ht="12.75" hidden="1">
+    <row r="48" spans="1:30" ht="12.75">
       <c r="A48" s="4">
         <v>22081193306</v>
       </c>
@@ -12691,7 +12691,7 @@
       <c r="AC48" s="3"/>
       <c r="AD48" s="3"/>
     </row>
-    <row r="49" spans="1:30" ht="12.75" hidden="1">
+    <row r="49" spans="1:30" ht="12.75">
       <c r="A49" s="4">
         <v>60481309986</v>
       </c>
@@ -12771,7 +12771,7 @@
       <c r="AC49" s="3"/>
       <c r="AD49" s="3"/>
     </row>
-    <row r="50" spans="1:30" ht="12.75" hidden="1">
+    <row r="50" spans="1:30" ht="12.75">
       <c r="A50" s="4">
         <v>50181000506</v>
       </c>
@@ -12851,7 +12851,7 @@
       <c r="AC50" s="3"/>
       <c r="AD50" s="3"/>
     </row>
-    <row r="51" spans="1:30" ht="12.75" hidden="1">
+    <row r="51" spans="1:30" ht="12.75">
       <c r="A51" s="4">
         <v>40881000286</v>
       </c>
@@ -12931,7 +12931,7 @@
       <c r="AC51" s="3"/>
       <c r="AD51" s="3"/>
     </row>
-    <row r="52" spans="1:30" ht="12.75" hidden="1">
+    <row r="52" spans="1:30" ht="12.75">
       <c r="A52" s="4">
         <v>60686257976</v>
       </c>
@@ -13011,7 +13011,7 @@
       <c r="AC52" s="3"/>
       <c r="AD52" s="3"/>
     </row>
-    <row r="53" spans="1:30" ht="12.75" hidden="1">
+    <row r="53" spans="1:30" ht="12.75">
       <c r="A53" s="4">
         <v>50681221566</v>
       </c>
@@ -13091,7 +13091,7 @@
       <c r="AC53" s="3"/>
       <c r="AD53" s="3"/>
     </row>
-    <row r="54" spans="1:30" ht="12.75" hidden="1">
+    <row r="54" spans="1:30" ht="12.75">
       <c r="A54" s="4">
         <v>61281322836</v>
       </c>
@@ -13171,7 +13171,7 @@
       <c r="AC54" s="3"/>
       <c r="AD54" s="3"/>
     </row>
-    <row r="55" spans="1:30" ht="12.75" hidden="1">
+    <row r="55" spans="1:30" ht="12.75">
       <c r="A55" s="4">
         <v>20686446676</v>
       </c>
@@ -13251,7 +13251,7 @@
       <c r="AC55" s="3"/>
       <c r="AD55" s="3"/>
     </row>
-    <row r="56" spans="1:30" ht="12.75" hidden="1">
+    <row r="56" spans="1:30" ht="12.75">
       <c r="A56" s="4">
         <v>13086571146</v>
       </c>
@@ -13331,7 +13331,7 @@
       <c r="AC56" s="3"/>
       <c r="AD56" s="3"/>
     </row>
-    <row r="57" spans="1:30" ht="12.75" hidden="1">
+    <row r="57" spans="1:30" ht="12.75">
       <c r="A57" s="4">
         <v>22086230666</v>
       </c>
@@ -13411,7 +13411,7 @@
       <c r="AC57" s="3"/>
       <c r="AD57" s="3"/>
     </row>
-    <row r="58" spans="1:30" ht="12.75" hidden="1">
+    <row r="58" spans="1:30" ht="12.75">
       <c r="A58" s="4">
         <v>61281306316</v>
       </c>
@@ -13489,7 +13489,7 @@
       <c r="AC58" s="3"/>
       <c r="AD58" s="3"/>
     </row>
-    <row r="59" spans="1:30" ht="12.75" hidden="1">
+    <row r="59" spans="1:30" ht="12.75">
       <c r="A59" s="4">
         <v>20181441586</v>
       </c>
@@ -13569,7 +13569,7 @@
       <c r="AC59" s="3"/>
       <c r="AD59" s="3"/>
     </row>
-    <row r="60" spans="1:30" ht="12.75" hidden="1">
+    <row r="60" spans="1:30" ht="12.75">
       <c r="A60" s="4">
         <v>10481181216</v>
       </c>
@@ -13649,7 +13649,7 @@
       <c r="AC60" s="3"/>
       <c r="AD60" s="3"/>
     </row>
-    <row r="61" spans="1:30" ht="12.75" hidden="1">
+    <row r="61" spans="1:30" ht="12.75">
       <c r="A61" s="4">
         <v>10781171936</v>
       </c>
@@ -13727,7 +13727,7 @@
       <c r="AC61" s="3"/>
       <c r="AD61" s="3"/>
     </row>
-    <row r="62" spans="1:30" ht="12.75" hidden="1">
+    <row r="62" spans="1:30" ht="12.75">
       <c r="A62" s="4">
         <v>62186083996</v>
       </c>
@@ -13807,7 +13807,7 @@
       <c r="AC62" s="3"/>
       <c r="AD62" s="3"/>
     </row>
-    <row r="63" spans="1:30" ht="12.75" hidden="1">
+    <row r="63" spans="1:30" ht="12.75">
       <c r="A63" s="4">
         <v>10481181216</v>
       </c>
@@ -13887,7 +13887,7 @@
       <c r="AC63" s="3"/>
       <c r="AD63" s="3"/>
     </row>
-    <row r="64" spans="1:30" ht="12.75" hidden="1">
+    <row r="64" spans="1:30" ht="12.75">
       <c r="A64" s="4">
         <v>10181349286</v>
       </c>
@@ -13967,7 +13967,7 @@
       <c r="AC64" s="3"/>
       <c r="AD64" s="3"/>
     </row>
-    <row r="65" spans="1:30" ht="12.75" hidden="1">
+    <row r="65" spans="1:30" ht="12.75">
       <c r="A65" s="4">
         <v>31281420716</v>
       </c>
@@ -14047,7 +14047,7 @@
       <c r="AC65" s="3"/>
       <c r="AD65" s="3"/>
     </row>
-    <row r="66" spans="1:30" ht="12.75" hidden="1">
+    <row r="66" spans="1:30" ht="12.75">
       <c r="A66" s="4">
         <v>60581755286</v>
       </c>
@@ -14125,7 +14125,7 @@
       <c r="AC66" s="3"/>
       <c r="AD66" s="3"/>
     </row>
-    <row r="67" spans="1:30" ht="12.75" hidden="1">
+    <row r="67" spans="1:30" ht="12.75">
       <c r="A67" s="4">
         <v>12381313726</v>
       </c>
@@ -14205,7 +14205,7 @@
       <c r="AC67" s="3"/>
       <c r="AD67" s="3"/>
     </row>
-    <row r="68" spans="1:30" ht="12.75" hidden="1">
+    <row r="68" spans="1:30" ht="12.75">
       <c r="A68" s="4">
         <v>20181456856</v>
       </c>
@@ -14285,7 +14285,7 @@
       <c r="AC68" s="3"/>
       <c r="AD68" s="3"/>
     </row>
-    <row r="69" spans="1:30" ht="12.75" hidden="1">
+    <row r="69" spans="1:30" ht="12.75">
       <c r="A69" s="4">
         <v>10186393126</v>
       </c>
@@ -14365,7 +14365,7 @@
       <c r="AC69" s="3"/>
       <c r="AD69" s="3"/>
     </row>
-    <row r="70" spans="1:30" ht="12.75" hidden="1">
+    <row r="70" spans="1:30" ht="12.75">
       <c r="A70" s="4">
         <v>31481079546</v>
       </c>
@@ -14445,7 +14445,7 @@
       <c r="AC70" s="3"/>
       <c r="AD70" s="3"/>
     </row>
-    <row r="71" spans="1:30" ht="12.75" hidden="1">
+    <row r="71" spans="1:30" ht="12.75">
       <c r="A71" s="4">
         <v>21188277766</v>
       </c>
@@ -14525,7 +14525,7 @@
       <c r="AC71" s="3"/>
       <c r="AD71" s="3"/>
     </row>
-    <row r="72" spans="1:30" ht="12.75" hidden="1">
+    <row r="72" spans="1:30" ht="12.75">
       <c r="A72" s="4">
         <v>60586231226</v>
       </c>
@@ -14605,7 +14605,7 @@
       <c r="AC72" s="3"/>
       <c r="AD72" s="3"/>
     </row>
-    <row r="73" spans="1:30" ht="12.75" hidden="1">
+    <row r="73" spans="1:30" ht="12.75">
       <c r="A73" s="4">
         <v>60586038446</v>
       </c>
@@ -14685,7 +14685,7 @@
       <c r="AC73" s="3"/>
       <c r="AD73" s="3"/>
     </row>
-    <row r="74" spans="1:30" ht="12.75" hidden="1">
+    <row r="74" spans="1:30" ht="12.75">
       <c r="A74" s="4">
         <v>10186234836</v>
       </c>
@@ -14765,7 +14765,7 @@
       <c r="AC74" s="3"/>
       <c r="AD74" s="3"/>
     </row>
-    <row r="75" spans="1:30" ht="12.75" hidden="1">
+    <row r="75" spans="1:30" ht="12.75">
       <c r="A75" s="4">
         <v>41081847876</v>
       </c>
@@ -14845,7 +14845,7 @@
       <c r="AC75" s="3"/>
       <c r="AD75" s="3"/>
     </row>
-    <row r="76" spans="1:30" ht="12.75" hidden="1">
+    <row r="76" spans="1:30" ht="12.75">
       <c r="A76" s="4">
         <v>11781568736</v>
       </c>
@@ -14925,7 +14925,7 @@
       <c r="AC76" s="3"/>
       <c r="AD76" s="3"/>
     </row>
-    <row r="77" spans="1:30" ht="12.75" hidden="1">
+    <row r="77" spans="1:30" ht="12.75">
       <c r="A77" s="4">
         <v>21481699656</v>
       </c>
@@ -15005,7 +15005,7 @@
       <c r="AC77" s="3"/>
       <c r="AD77" s="3"/>
     </row>
-    <row r="78" spans="1:30" ht="12.75" hidden="1">
+    <row r="78" spans="1:30" ht="12.75">
       <c r="A78" s="4">
         <v>61381098256</v>
       </c>
@@ -15085,7 +15085,7 @@
       <c r="AC78" s="3"/>
       <c r="AD78" s="3"/>
     </row>
-    <row r="79" spans="1:30" ht="12.75" hidden="1">
+    <row r="79" spans="1:30" ht="12.75">
       <c r="A79" s="4">
         <v>40981312766</v>
       </c>
@@ -15165,7 +15165,7 @@
       <c r="AC79" s="3"/>
       <c r="AD79" s="3"/>
     </row>
-    <row r="80" spans="1:30" ht="12.75" hidden="1">
+    <row r="80" spans="1:30" ht="12.75">
       <c r="A80" s="4">
         <v>90706263127</v>
       </c>
@@ -15245,7 +15245,7 @@
       <c r="AC80" s="3"/>
       <c r="AD80" s="3"/>
     </row>
-    <row r="81" spans="1:30" ht="12.75" hidden="1">
+    <row r="81" spans="1:30" ht="12.75">
       <c r="A81" s="4">
         <v>62181650896</v>
       </c>
@@ -15323,7 +15323,7 @@
       <c r="AC81" s="3"/>
       <c r="AD81" s="3"/>
     </row>
-    <row r="82" spans="1:30" ht="12.75" hidden="1">
+    <row r="82" spans="1:30" ht="12.75">
       <c r="A82" s="4">
         <v>13081281806</v>
       </c>
@@ -15403,7 +15403,7 @@
       <c r="AC82" s="3"/>
       <c r="AD82" s="3"/>
     </row>
-    <row r="83" spans="1:30" ht="12.75" hidden="1">
+    <row r="83" spans="1:30" ht="12.75">
       <c r="A83" s="4">
         <v>10581296406</v>
       </c>
@@ -15479,7 +15479,7 @@
       <c r="AC83" s="3"/>
       <c r="AD83" s="3"/>
     </row>
-    <row r="84" spans="1:30" ht="12.75" hidden="1">
+    <row r="84" spans="1:30" ht="12.75">
       <c r="A84" s="4">
         <v>62181407736</v>
       </c>
@@ -15559,7 +15559,7 @@
       <c r="AC84" s="3"/>
       <c r="AD84" s="3"/>
     </row>
-    <row r="85" spans="1:30" ht="12.75" hidden="1">
+    <row r="85" spans="1:30" ht="12.75">
       <c r="A85" s="4">
         <v>10788089036</v>
       </c>
@@ -15639,7 +15639,7 @@
       <c r="AC85" s="3"/>
       <c r="AD85" s="3"/>
     </row>
-    <row r="86" spans="1:30" ht="12.75" hidden="1">
+    <row r="86" spans="1:30" ht="12.75">
       <c r="A86" s="4">
         <v>10786453366</v>
       </c>
@@ -15719,7 +15719,7 @@
       <c r="AC86" s="3"/>
       <c r="AD86" s="3"/>
     </row>
-    <row r="87" spans="1:30" ht="12.75" hidden="1">
+    <row r="87" spans="1:30" ht="12.75">
       <c r="A87" s="4">
         <v>12386356936</v>
       </c>
@@ -15799,7 +15799,7 @@
       <c r="AC87" s="3"/>
       <c r="AD87" s="3"/>
     </row>
-    <row r="88" spans="1:30" ht="12.75" hidden="1">
+    <row r="88" spans="1:30" ht="12.75">
       <c r="A88" s="4">
         <v>40381132706</v>
       </c>
@@ -15879,7 +15879,7 @@
       <c r="AC88" s="3"/>
       <c r="AD88" s="3"/>
     </row>
-    <row r="89" spans="1:30" ht="12.75" hidden="1">
+    <row r="89" spans="1:30" ht="12.75">
       <c r="A89" s="4">
         <v>31481079546</v>
       </c>
@@ -15959,7 +15959,7 @@
       <c r="AC89" s="3"/>
       <c r="AD89" s="3"/>
     </row>
-    <row r="90" spans="1:30" ht="12.75" hidden="1">
+    <row r="90" spans="1:30" ht="12.75">
       <c r="A90" s="4">
         <v>10581595196</v>
       </c>
@@ -16039,7 +16039,7 @@
       <c r="AC90" s="3"/>
       <c r="AD90" s="3"/>
     </row>
-    <row r="91" spans="1:30" ht="12.75" hidden="1">
+    <row r="91" spans="1:30" ht="12.75">
       <c r="A91" s="4">
         <v>26481026356</v>
       </c>
@@ -16119,7 +16119,7 @@
       <c r="AC91" s="3"/>
       <c r="AD91" s="3"/>
     </row>
-    <row r="92" spans="1:30" ht="12.75" hidden="1">
+    <row r="92" spans="1:30" ht="12.75">
       <c r="A92" s="4">
         <v>22981197736</v>
       </c>
@@ -16199,7 +16199,7 @@
       <c r="AC92" s="3"/>
       <c r="AD92" s="3"/>
     </row>
-    <row r="93" spans="1:30" ht="12.75" hidden="1">
+    <row r="93" spans="1:30" ht="12.75">
       <c r="A93" s="4">
         <v>31681240416</v>
       </c>
@@ -16279,7 +16279,7 @@
       <c r="AC93" s="3"/>
       <c r="AD93" s="3"/>
     </row>
-    <row r="94" spans="1:30" ht="12.75" hidden="1">
+    <row r="94" spans="1:30" ht="12.75">
       <c r="A94" s="4">
         <v>31681240416</v>
       </c>
@@ -16359,7 +16359,7 @@
       <c r="AC94" s="3"/>
       <c r="AD94" s="3"/>
     </row>
-    <row r="95" spans="1:30" ht="12.75" hidden="1">
+    <row r="95" spans="1:30" ht="12.75">
       <c r="A95" s="4">
         <v>31681240416</v>
       </c>
@@ -16439,7 +16439,7 @@
       <c r="AC95" s="3"/>
       <c r="AD95" s="3"/>
     </row>
-    <row r="96" spans="1:30" ht="12.75" hidden="1">
+    <row r="96" spans="1:30" ht="12.75">
       <c r="A96" s="4">
         <v>22081193306</v>
       </c>
@@ -16519,7 +16519,7 @@
       <c r="AC96" s="3"/>
       <c r="AD96" s="3"/>
     </row>
-    <row r="97" spans="1:30" ht="12.75" hidden="1">
+    <row r="97" spans="1:30" ht="12.75">
       <c r="A97" s="4">
         <v>11481588536</v>
       </c>
@@ -16599,7 +16599,7 @@
       <c r="AC97" s="3"/>
       <c r="AD97" s="3"/>
     </row>
-    <row r="98" spans="1:30" ht="12.75" hidden="1">
+    <row r="98" spans="1:30" ht="12.75">
       <c r="A98" s="4">
         <v>37087002016</v>
       </c>
@@ -16679,7 +16679,7 @@
       <c r="AC98" s="3"/>
       <c r="AD98" s="3"/>
     </row>
-    <row r="99" spans="1:30" ht="12.75" hidden="1">
+    <row r="99" spans="1:30" ht="12.75">
       <c r="A99" s="4">
         <v>90708487507</v>
       </c>
@@ -16759,7 +16759,7 @@
       <c r="AC99" s="3"/>
       <c r="AD99" s="3"/>
     </row>
-    <row r="100" spans="1:30" ht="12.75" hidden="1">
+    <row r="100" spans="1:30" ht="12.75">
       <c r="A100" s="4">
         <v>20181310276</v>
       </c>
@@ -16839,7 +16839,7 @@
       <c r="AC100" s="3"/>
       <c r="AD100" s="3"/>
     </row>
-    <row r="101" spans="1:30" ht="12.75" hidden="1">
+    <row r="101" spans="1:30" ht="12.75">
       <c r="A101" s="4">
         <v>10181162936</v>
       </c>
@@ -16919,7 +16919,7 @@
       <c r="AC101" s="3"/>
       <c r="AD101" s="3"/>
     </row>
-    <row r="102" spans="1:30" ht="12.75" hidden="1">
+    <row r="102" spans="1:30" ht="12.75">
       <c r="A102" s="4">
         <v>90700104187</v>
       </c>
@@ -16999,7 +16999,7 @@
       <c r="AC102" s="3"/>
       <c r="AD102" s="3"/>
     </row>
-    <row r="103" spans="1:30" ht="12.75" hidden="1">
+    <row r="103" spans="1:30" ht="12.75">
       <c r="A103" s="4">
         <v>50386167766</v>
       </c>
@@ -17079,7 +17079,7 @@
       <c r="AC103" s="3"/>
       <c r="AD103" s="3"/>
     </row>
-    <row r="104" spans="1:30" ht="12.75" hidden="1">
+    <row r="104" spans="1:30" ht="12.75">
       <c r="A104" s="4">
         <v>11081146116</v>
       </c>
@@ -17159,7 +17159,7 @@
       <c r="AC104" s="3"/>
       <c r="AD104" s="3"/>
     </row>
-    <row r="105" spans="1:30" ht="12.75" hidden="1">
+    <row r="105" spans="1:30" ht="12.75">
       <c r="A105" s="4">
         <v>31681240416</v>
       </c>
@@ -17239,7 +17239,7 @@
       <c r="AC105" s="3"/>
       <c r="AD105" s="3"/>
     </row>
-    <row r="106" spans="1:30" ht="12.75" hidden="1">
+    <row r="106" spans="1:30" ht="12.75">
       <c r="A106" s="4">
         <v>60481181796</v>
       </c>
@@ -17319,7 +17319,7 @@
       <c r="AC106" s="3"/>
       <c r="AD106" s="3"/>
     </row>
-    <row r="107" spans="1:30" ht="12.75" hidden="1">
+    <row r="107" spans="1:30" ht="12.75">
       <c r="A107" s="4">
         <v>61581000106</v>
       </c>
@@ -17397,7 +17397,7 @@
       <c r="AC107" s="3"/>
       <c r="AD107" s="3"/>
     </row>
-    <row r="108" spans="1:30" ht="12.75" hidden="1">
+    <row r="108" spans="1:30" ht="12.75">
       <c r="A108" s="4">
         <v>12001602216</v>
       </c>
@@ -17477,7 +17477,7 @@
       <c r="AC108" s="3"/>
       <c r="AD108" s="3"/>
     </row>
-    <row r="109" spans="1:30" ht="12.75" hidden="1">
+    <row r="109" spans="1:30" ht="12.75">
       <c r="A109" s="4">
         <v>20181441586</v>
       </c>
@@ -17557,7 +17557,7 @@
       <c r="AC109" s="3"/>
       <c r="AD109" s="3"/>
     </row>
-    <row r="110" spans="1:30" ht="12.75" hidden="1">
+    <row r="110" spans="1:30" ht="12.75">
       <c r="A110" s="4">
         <v>33586000796</v>
       </c>
@@ -17637,7 +17637,7 @@
       <c r="AC110" s="3"/>
       <c r="AD110" s="3"/>
     </row>
-    <row r="111" spans="1:30" ht="12.75" hidden="1">
+    <row r="111" spans="1:30" ht="12.75">
       <c r="A111" s="4">
         <v>21481699656</v>
       </c>
@@ -17717,7 +17717,7 @@
       <c r="AC111" s="3"/>
       <c r="AD111" s="3"/>
     </row>
-    <row r="112" spans="1:30" ht="12.75" hidden="1">
+    <row r="112" spans="1:30" ht="12.75">
       <c r="A112" s="4">
         <v>35981003096</v>
       </c>
@@ -17797,7 +17797,7 @@
       <c r="AC112" s="3"/>
       <c r="AD112" s="3"/>
     </row>
-    <row r="113" spans="1:30" ht="12.75" hidden="1">
+    <row r="113" spans="1:30" ht="12.75">
       <c r="A113" s="4">
         <v>11681350076</v>
       </c>
@@ -17877,7 +17877,7 @@
       <c r="AC113" s="3"/>
       <c r="AD113" s="3"/>
     </row>
-    <row r="114" spans="1:30" ht="12.75" hidden="1">
+    <row r="114" spans="1:30" ht="12.75">
       <c r="A114" s="4">
         <v>22481113976</v>
       </c>
@@ -17957,7 +17957,7 @@
       <c r="AC114" s="3"/>
       <c r="AD114" s="3"/>
     </row>
-    <row r="115" spans="1:30" ht="12.75" hidden="1">
+    <row r="115" spans="1:30" ht="12.75">
       <c r="A115" s="4">
         <v>41781128486</v>
       </c>
@@ -18037,7 +18037,7 @@
       <c r="AC115" s="3"/>
       <c r="AD115" s="3"/>
     </row>
-    <row r="116" spans="1:30" ht="12.75" hidden="1">
+    <row r="116" spans="1:30" ht="12.75">
       <c r="A116" s="4">
         <v>14081914156</v>
       </c>
@@ -18117,7 +18117,7 @@
       <c r="AC116" s="3"/>
       <c r="AD116" s="3"/>
     </row>
-    <row r="117" spans="1:30" ht="12.75" hidden="1">
+    <row r="117" spans="1:30" ht="12.75">
       <c r="A117" s="4">
         <v>10481181216</v>
       </c>
@@ -18197,7 +18197,7 @@
       <c r="AC117" s="3"/>
       <c r="AD117" s="3"/>
     </row>
-    <row r="118" spans="1:30" ht="12.75" hidden="1">
+    <row r="118" spans="1:30" ht="12.75">
       <c r="A118" s="4">
         <v>41181457736</v>
       </c>
@@ -18277,7 +18277,7 @@
       <c r="AC118" s="3"/>
       <c r="AD118" s="3"/>
     </row>
-    <row r="119" spans="1:30" ht="12.75" hidden="1">
+    <row r="119" spans="1:30" ht="12.75">
       <c r="A119" s="4">
         <v>21781164866</v>
       </c>
@@ -18357,7 +18357,7 @@
       <c r="AC119" s="3"/>
       <c r="AD119" s="3"/>
     </row>
-    <row r="120" spans="1:30" ht="12.75" hidden="1">
+    <row r="120" spans="1:30" ht="12.75">
       <c r="A120" s="4">
         <v>21781164866</v>
       </c>
@@ -18437,7 +18437,7 @@
       <c r="AC120" s="3"/>
       <c r="AD120" s="3"/>
     </row>
-    <row r="121" spans="1:30" ht="12.75" hidden="1">
+    <row r="121" spans="1:30" ht="12.75">
       <c r="A121" s="4">
         <v>21586286236</v>
       </c>
@@ -18517,7 +18517,7 @@
       <c r="AC121" s="3"/>
       <c r="AD121" s="3"/>
     </row>
-    <row r="122" spans="1:30" ht="12.75" hidden="1">
+    <row r="122" spans="1:30" ht="12.75">
       <c r="A122" s="4">
         <v>61581181316</v>
       </c>
@@ -18595,7 +18595,7 @@
       <c r="AC122" s="3"/>
       <c r="AD122" s="3"/>
     </row>
-    <row r="123" spans="1:30" ht="12.75" hidden="1">
+    <row r="123" spans="1:30" ht="12.75">
       <c r="A123" s="4">
         <v>60381255996</v>
       </c>
@@ -18675,7 +18675,7 @@
       <c r="AC123" s="3"/>
       <c r="AD123" s="3"/>
     </row>
-    <row r="124" spans="1:30" ht="12.75" hidden="1">
+    <row r="124" spans="1:30" ht="12.75">
       <c r="A124" s="4">
         <v>22481113976</v>
       </c>
@@ -18755,7 +18755,7 @@
       <c r="AC124" s="3"/>
       <c r="AD124" s="3"/>
     </row>
-    <row r="125" spans="1:30" ht="12.75" hidden="1">
+    <row r="125" spans="1:30" ht="12.75">
       <c r="A125" s="4">
         <v>30781066896</v>
       </c>
@@ -18835,7 +18835,7 @@
       <c r="AC125" s="3"/>
       <c r="AD125" s="3"/>
     </row>
-    <row r="126" spans="1:30" ht="12.75" hidden="1">
+    <row r="126" spans="1:30" ht="12.75">
       <c r="A126" s="4">
         <v>60781330726</v>
       </c>
@@ -18915,7 +18915,7 @@
       <c r="AC126" s="3"/>
       <c r="AD126" s="3"/>
     </row>
-    <row r="127" spans="1:30" ht="12.75" hidden="1">
+    <row r="127" spans="1:30" ht="12.75">
       <c r="A127" s="4">
         <v>10481181216</v>
       </c>
@@ -18995,7 +18995,7 @@
       <c r="AC127" s="3"/>
       <c r="AD127" s="3"/>
     </row>
-    <row r="128" spans="1:30" ht="12.75" hidden="1">
+    <row r="128" spans="1:30" ht="12.75">
       <c r="A128" s="4">
         <v>10186234836</v>
       </c>
@@ -19075,7 +19075,7 @@
       <c r="AC128" s="3"/>
       <c r="AD128" s="3"/>
     </row>
-    <row r="129" spans="1:30" ht="12.75" hidden="1">
+    <row r="129" spans="1:30" ht="12.75">
       <c r="A129" s="4">
         <v>14281016186</v>
       </c>
@@ -19155,7 +19155,7 @@
       <c r="AC129" s="3"/>
       <c r="AD129" s="3"/>
     </row>
-    <row r="130" spans="1:30" ht="12.75" hidden="1">
+    <row r="130" spans="1:30" ht="12.75">
       <c r="A130" s="4">
         <v>22081124676</v>
       </c>
@@ -19235,7 +19235,7 @@
       <c r="AC130" s="3"/>
       <c r="AD130" s="3"/>
     </row>
-    <row r="131" spans="1:30" ht="12.75" hidden="1">
+    <row r="131" spans="1:30" ht="12.75">
       <c r="A131" s="4">
         <v>90708487507</v>
       </c>
@@ -19315,7 +19315,7 @@
       <c r="AC131" s="3"/>
       <c r="AD131" s="3"/>
     </row>
-    <row r="132" spans="1:30" ht="12.75" hidden="1">
+    <row r="132" spans="1:30" ht="12.75">
       <c r="A132" s="4">
         <v>21081503006</v>
       </c>
@@ -19395,7 +19395,7 @@
       <c r="AC132" s="3"/>
       <c r="AD132" s="3"/>
     </row>
-    <row r="133" spans="1:30" ht="12.75" hidden="1">
+    <row r="133" spans="1:30" ht="12.75">
       <c r="A133" s="4">
         <v>40886116466</v>
       </c>
@@ -19475,7 +19475,7 @@
       <c r="AC133" s="3"/>
       <c r="AD133" s="3"/>
     </row>
-    <row r="134" spans="1:30" ht="12.75" hidden="1">
+    <row r="134" spans="1:30" ht="12.75">
       <c r="A134" s="4">
         <v>50681762206</v>
       </c>
@@ -19555,7 +19555,7 @@
       <c r="AC134" s="3"/>
       <c r="AD134" s="3"/>
     </row>
-    <row r="135" spans="1:30" ht="12.75" hidden="1">
+    <row r="135" spans="1:30" ht="12.75">
       <c r="A135" s="4">
         <v>13481824206</v>
       </c>
@@ -19635,7 +19635,7 @@
       <c r="AC135" s="3"/>
       <c r="AD135" s="3"/>
     </row>
-    <row r="136" spans="1:30" ht="12.75" hidden="1">
+    <row r="136" spans="1:30" ht="12.75">
       <c r="A136" s="4">
         <v>61781042876</v>
       </c>
@@ -19715,7 +19715,7 @@
       <c r="AC136" s="3"/>
       <c r="AD136" s="3"/>
     </row>
-    <row r="137" spans="1:30" ht="12.75" hidden="1">
+    <row r="137" spans="1:30" ht="12.75">
       <c r="A137" s="4">
         <v>11781495766</v>
       </c>
@@ -19795,7 +19795,7 @@
       <c r="AC137" s="3"/>
       <c r="AD137" s="3"/>
     </row>
-    <row r="138" spans="1:30" ht="12.75" hidden="1">
+    <row r="138" spans="1:30" ht="12.75">
       <c r="A138" s="4">
         <v>41681719946</v>
       </c>
@@ -19875,7 +19875,7 @@
       <c r="AC138" s="3"/>
       <c r="AD138" s="3"/>
     </row>
-    <row r="139" spans="1:30" ht="12.75" hidden="1">
+    <row r="139" spans="1:30" ht="12.75">
       <c r="A139" s="4">
         <v>20181441586</v>
       </c>
@@ -19955,7 +19955,7 @@
       <c r="AC139" s="3"/>
       <c r="AD139" s="3"/>
     </row>
-    <row r="140" spans="1:30" ht="12.75" hidden="1">
+    <row r="140" spans="1:30" ht="12.75">
       <c r="A140" s="4">
         <v>21186432816</v>
       </c>
@@ -20035,7 +20035,7 @@
       <c r="AC140" s="3"/>
       <c r="AD140" s="3"/>
     </row>
-    <row r="141" spans="1:30" ht="12.75" hidden="1">
+    <row r="141" spans="1:30" ht="12.75">
       <c r="A141" s="4">
         <v>50881147596</v>
       </c>
@@ -20115,7 +20115,7 @@
       <c r="AC141" s="3"/>
       <c r="AD141" s="3"/>
     </row>
-    <row r="142" spans="1:30" ht="12.75" hidden="1">
+    <row r="142" spans="1:30" ht="12.75">
       <c r="A142" s="4">
         <v>10481734066</v>
       </c>
@@ -20195,7 +20195,7 @@
       <c r="AC142" s="3"/>
       <c r="AD142" s="3"/>
     </row>
-    <row r="143" spans="1:30" ht="12.75" hidden="1">
+    <row r="143" spans="1:30" ht="12.75">
       <c r="A143" s="4">
         <v>22086230666</v>
       </c>
@@ -20275,7 +20275,7 @@
       <c r="AC143" s="3"/>
       <c r="AD143" s="3"/>
     </row>
-    <row r="144" spans="1:30" ht="12.75" hidden="1">
+    <row r="144" spans="1:30" ht="12.75">
       <c r="A144" s="4">
         <v>62181431786</v>
       </c>
@@ -20355,7 +20355,7 @@
       <c r="AC144" s="3"/>
       <c r="AD144" s="3"/>
     </row>
-    <row r="145" spans="1:30" ht="12.75" hidden="1">
+    <row r="145" spans="1:30" ht="12.75">
       <c r="A145" s="4">
         <v>31581051916</v>
       </c>
@@ -20435,7 +20435,7 @@
       <c r="AC145" s="3"/>
       <c r="AD145" s="3"/>
     </row>
-    <row r="146" spans="1:30" ht="12.75" hidden="1">
+    <row r="146" spans="1:30" ht="12.75">
       <c r="A146" s="4">
         <v>40881602206</v>
       </c>
@@ -20515,7 +20515,7 @@
       <c r="AC146" s="3"/>
       <c r="AD146" s="3"/>
     </row>
-    <row r="147" spans="1:30" ht="12.75" hidden="1">
+    <row r="147" spans="1:30" ht="12.75">
       <c r="A147" s="4">
         <v>51381039296</v>
       </c>
@@ -20595,7 +20595,7 @@
       <c r="AC147" s="3"/>
       <c r="AD147" s="3"/>
     </row>
-    <row r="148" spans="1:30" ht="12.75" hidden="1">
+    <row r="148" spans="1:30" ht="12.75">
       <c r="A148" s="4">
         <v>21481699656</v>
       </c>
@@ -20675,7 +20675,7 @@
       <c r="AC148" s="3"/>
       <c r="AD148" s="3"/>
     </row>
-    <row r="149" spans="1:30" ht="12.75" hidden="1">
+    <row r="149" spans="1:30" ht="12.75">
       <c r="A149" s="4">
         <v>13081541506</v>
       </c>
@@ -20755,7 +20755,7 @@
       <c r="AC149" s="3"/>
       <c r="AD149" s="3"/>
     </row>
-    <row r="150" spans="1:30" ht="12.75" hidden="1">
+    <row r="150" spans="1:30" ht="12.75">
       <c r="A150" s="4">
         <v>11481588536</v>
       </c>
@@ -20835,7 +20835,7 @@
       <c r="AC150" s="3"/>
       <c r="AD150" s="3"/>
     </row>
-    <row r="151" spans="1:30" ht="12.75" hidden="1">
+    <row r="151" spans="1:30" ht="12.75">
       <c r="A151" s="4">
         <v>41081847876</v>
       </c>
@@ -20915,7 +20915,7 @@
       <c r="AC151" s="3"/>
       <c r="AD151" s="3"/>
     </row>
-    <row r="152" spans="1:30" ht="12.75" hidden="1">
+    <row r="152" spans="1:30" ht="12.75">
       <c r="A152" s="4">
         <v>22081193306</v>
       </c>
@@ -20995,7 +20995,7 @@
       <c r="AC152" s="3"/>
       <c r="AD152" s="3"/>
     </row>
-    <row r="153" spans="1:30" ht="12.75" hidden="1">
+    <row r="153" spans="1:30" ht="12.75">
       <c r="A153" s="4">
         <v>11481588536</v>
       </c>
@@ -21075,7 +21075,7 @@
       <c r="AC153" s="3"/>
       <c r="AD153" s="3"/>
     </row>
-    <row r="154" spans="1:30" ht="12.75" hidden="1">
+    <row r="154" spans="1:30" ht="12.75">
       <c r="A154" s="4">
         <v>62081465326</v>
       </c>
@@ -21155,7 +21155,7 @@
       <c r="AC154" s="3"/>
       <c r="AD154" s="3"/>
     </row>
-    <row r="155" spans="1:30" ht="12.75" hidden="1">
+    <row r="155" spans="1:30" ht="12.75">
       <c r="A155" s="4">
         <v>41086447236</v>
       </c>
@@ -21235,7 +21235,7 @@
       <c r="AC155" s="3"/>
       <c r="AD155" s="3"/>
     </row>
-    <row r="156" spans="1:30" ht="12.75" hidden="1">
+    <row r="156" spans="1:30" ht="12.75">
       <c r="A156" s="4">
         <v>13486592786</v>
       </c>
@@ -21315,7 +21315,7 @@
       <c r="AC156" s="3"/>
       <c r="AD156" s="3"/>
     </row>
-    <row r="157" spans="1:30" ht="12.75" hidden="1">
+    <row r="157" spans="1:30" ht="12.75">
       <c r="A157" s="4">
         <v>11481588536</v>
       </c>
@@ -21395,7 +21395,7 @@
       <c r="AC157" s="3"/>
       <c r="AD157" s="3"/>
     </row>
-    <row r="158" spans="1:30" ht="12.75" hidden="1">
+    <row r="158" spans="1:30" ht="12.75">
       <c r="A158" s="4">
         <v>31481304366</v>
       </c>
@@ -21475,7 +21475,7 @@
       <c r="AC158" s="3"/>
       <c r="AD158" s="3"/>
     </row>
-    <row r="159" spans="1:30" ht="12.75" hidden="1">
+    <row r="159" spans="1:30" ht="12.75">
       <c r="A159" s="4">
         <v>11681350076</v>
       </c>
@@ -21555,7 +21555,7 @@
       <c r="AC159" s="3"/>
       <c r="AD159" s="3"/>
     </row>
-    <row r="160" spans="1:30" ht="12.75" hidden="1">
+    <row r="160" spans="1:30" ht="12.75">
       <c r="A160" s="4">
         <v>61381026526</v>
       </c>
@@ -21635,7 +21635,7 @@
       <c r="AC160" s="3"/>
       <c r="AD160" s="3"/>
     </row>
-    <row r="161" spans="1:30" ht="12.75" hidden="1">
+    <row r="161" spans="1:30" ht="12.75">
       <c r="A161" s="4">
         <v>10986531096</v>
       </c>
@@ -21715,7 +21715,7 @@
       <c r="AC161" s="3"/>
       <c r="AD161" s="3"/>
     </row>
-    <row r="162" spans="1:30" ht="12.75" hidden="1">
+    <row r="162" spans="1:30" ht="12.75">
       <c r="A162" s="4">
         <v>30181274596</v>
       </c>
@@ -21795,7 +21795,7 @@
       <c r="AC162" s="3"/>
       <c r="AD162" s="3"/>
     </row>
-    <row r="163" spans="1:30" ht="12.75" hidden="1">
+    <row r="163" spans="1:30" ht="12.75">
       <c r="A163" s="4">
         <v>90718336637</v>
       </c>
@@ -21875,7 +21875,7 @@
       <c r="AC163" s="3"/>
       <c r="AD163" s="3"/>
     </row>
-    <row r="164" spans="1:30" ht="12.75" hidden="1">
+    <row r="164" spans="1:30" ht="12.75">
       <c r="A164" s="4">
         <v>13881017736</v>
       </c>
@@ -21955,7 +21955,7 @@
       <c r="AC164" s="3"/>
       <c r="AD164" s="3"/>
     </row>
-    <row r="165" spans="1:30" ht="12.75" hidden="1">
+    <row r="165" spans="1:30" ht="12.75">
       <c r="A165" s="4">
         <v>13181544926</v>
       </c>
@@ -22035,7 +22035,7 @@
       <c r="AC165" s="3"/>
       <c r="AD165" s="3"/>
     </row>
-    <row r="166" spans="1:30" ht="12.75" hidden="1">
+    <row r="166" spans="1:30" ht="12.75">
       <c r="A166" s="4">
         <v>90700012517</v>
       </c>
@@ -22115,7 +22115,7 @@
       <c r="AC166" s="3"/>
       <c r="AD166" s="3"/>
     </row>
-    <row r="167" spans="1:30" ht="12.75" hidden="1">
+    <row r="167" spans="1:30" ht="12.75">
       <c r="A167" s="4">
         <v>41281097516</v>
       </c>
@@ -22193,7 +22193,7 @@
       <c r="AC167" s="3"/>
       <c r="AD167" s="3"/>
     </row>
-    <row r="168" spans="1:30" ht="12.75" hidden="1">
+    <row r="168" spans="1:30" ht="12.75">
       <c r="A168" s="4">
         <v>12886880266</v>
       </c>
@@ -22273,7 +22273,7 @@
       <c r="AC168" s="3"/>
       <c r="AD168" s="3"/>
     </row>
-    <row r="169" spans="1:30" ht="12.75" hidden="1">
+    <row r="169" spans="1:30" ht="12.75">
       <c r="A169" s="4">
         <v>61281025906</v>
       </c>
@@ -22351,7 +22351,7 @@
       <c r="AC169" s="3"/>
       <c r="AD169" s="3"/>
     </row>
-    <row r="170" spans="1:30" ht="12.75" hidden="1">
+    <row r="170" spans="1:30" ht="12.75">
       <c r="A170" s="4">
         <v>60881045516</v>
       </c>
@@ -22431,7 +22431,7 @@
       <c r="AC170" s="3"/>
       <c r="AD170" s="3"/>
     </row>
-    <row r="171" spans="1:30" ht="12.75" hidden="1">
+    <row r="171" spans="1:30" ht="12.75">
       <c r="A171" s="4">
         <v>12081951736</v>
       </c>
@@ -22511,7 +22511,7 @@
       <c r="AC171" s="3"/>
       <c r="AD171" s="3"/>
     </row>
-    <row r="172" spans="1:30" ht="12.75" hidden="1">
+    <row r="172" spans="1:30" ht="12.75">
       <c r="A172" s="4">
         <v>13681120516</v>
       </c>
@@ -22591,7 +22591,7 @@
       <c r="AC172" s="3"/>
       <c r="AD172" s="3"/>
     </row>
-    <row r="173" spans="1:30" ht="12.75" hidden="1">
+    <row r="173" spans="1:30" ht="12.75">
       <c r="A173" s="4">
         <v>21481994886</v>
       </c>
@@ -22671,7 +22671,7 @@
       <c r="AC173" s="3"/>
       <c r="AD173" s="3"/>
     </row>
-    <row r="174" spans="1:30" ht="12.75" hidden="1">
+    <row r="174" spans="1:30" ht="12.75">
       <c r="A174" s="4">
         <v>50681022806</v>
       </c>
@@ -22751,7 +22751,7 @@
       <c r="AC174" s="3"/>
       <c r="AD174" s="3"/>
     </row>
-    <row r="175" spans="1:30" ht="12.75" hidden="1">
+    <row r="175" spans="1:30" ht="12.75">
       <c r="A175" s="4">
         <v>20181441586</v>
       </c>
@@ -22831,7 +22831,7 @@
       <c r="AC175" s="3"/>
       <c r="AD175" s="3"/>
     </row>
-    <row r="176" spans="1:30" ht="12.75" hidden="1">
+    <row r="176" spans="1:30" ht="12.75">
       <c r="A176" s="4">
         <v>50881001776</v>
       </c>
@@ -22911,7 +22911,7 @@
       <c r="AC176" s="3"/>
       <c r="AD176" s="3"/>
     </row>
-    <row r="177" spans="1:30" ht="12.75" hidden="1">
+    <row r="177" spans="1:30" ht="12.75">
       <c r="A177" s="4">
         <v>50881001776</v>
       </c>
@@ -22991,7 +22991,7 @@
       <c r="AC177" s="3"/>
       <c r="AD177" s="3"/>
     </row>
-    <row r="178" spans="1:30" ht="12.75" hidden="1">
+    <row r="178" spans="1:30" ht="12.75">
       <c r="A178" s="4">
         <v>10181349286</v>
       </c>
@@ -23071,7 +23071,7 @@
       <c r="AC178" s="3"/>
       <c r="AD178" s="3"/>
     </row>
-    <row r="179" spans="1:30" ht="12.75" hidden="1">
+    <row r="179" spans="1:30" ht="12.75">
       <c r="A179" s="4">
         <v>10481181216</v>
       </c>
@@ -23151,7 +23151,7 @@
       <c r="AC179" s="3"/>
       <c r="AD179" s="3"/>
     </row>
-    <row r="180" spans="1:30" ht="12.75" hidden="1">
+    <row r="180" spans="1:30" ht="12.75">
       <c r="A180" s="4">
         <v>12681053256</v>
       </c>
@@ -23231,7 +23231,7 @@
       <c r="AC180" s="3"/>
       <c r="AD180" s="3"/>
     </row>
-    <row r="181" spans="1:30" ht="12.75" hidden="1">
+    <row r="181" spans="1:30" ht="12.75">
       <c r="A181" s="4">
         <v>12681053256</v>
       </c>
@@ -23311,7 +23311,7 @@
       <c r="AC181" s="3"/>
       <c r="AD181" s="3"/>
     </row>
-    <row r="182" spans="1:30" ht="12.75" hidden="1">
+    <row r="182" spans="1:30" ht="12.75">
       <c r="A182" s="4">
         <v>90708487507</v>
       </c>
@@ -23391,7 +23391,7 @@
       <c r="AC182" s="3"/>
       <c r="AD182" s="3"/>
     </row>
-    <row r="183" spans="1:30" ht="12.75" hidden="1">
+    <row r="183" spans="1:30" ht="12.75">
       <c r="A183" s="4">
         <v>40881000286</v>
       </c>
@@ -23471,7 +23471,7 @@
       <c r="AC183" s="3"/>
       <c r="AD183" s="3"/>
     </row>
-    <row r="184" spans="1:30" ht="12.75" hidden="1">
+    <row r="184" spans="1:30" ht="12.75">
       <c r="A184" s="4">
         <v>61781136226</v>
       </c>
@@ -23551,7 +23551,7 @@
       <c r="AC184" s="3"/>
       <c r="AD184" s="3"/>
     </row>
-    <row r="185" spans="1:30" ht="12.75" hidden="1">
+    <row r="185" spans="1:30" ht="12.75">
       <c r="A185" s="4">
         <v>40381132706</v>
       </c>
@@ -23631,7 +23631,7 @@
       <c r="AC185" s="3"/>
       <c r="AD185" s="3"/>
     </row>
-    <row r="186" spans="1:30" ht="12.75" hidden="1">
+    <row r="186" spans="1:30" ht="12.75">
       <c r="A186" s="4">
         <v>50681022806</v>
       </c>
@@ -23711,7 +23711,7 @@
       <c r="AC186" s="3"/>
       <c r="AD186" s="3"/>
     </row>
-    <row r="187" spans="1:30" ht="12.75" hidden="1">
+    <row r="187" spans="1:30" ht="12.75">
       <c r="A187" s="4">
         <v>21586089906</v>
       </c>
@@ -23791,7 +23791,7 @@
       <c r="AC187" s="3"/>
       <c r="AD187" s="3"/>
     </row>
-    <row r="188" spans="1:30" ht="12.75" hidden="1">
+    <row r="188" spans="1:30" ht="12.75">
       <c r="A188" s="4">
         <v>13581543636</v>
       </c>
@@ -23871,7 +23871,7 @@
       <c r="AC188" s="3"/>
       <c r="AD188" s="3"/>
     </row>
-    <row r="189" spans="1:30" ht="12.75" hidden="1">
+    <row r="189" spans="1:30" ht="12.75">
       <c r="A189" s="4">
         <v>60781179226</v>
       </c>
@@ -23951,7 +23951,7 @@
       <c r="AC189" s="3"/>
       <c r="AD189" s="3"/>
     </row>
-    <row r="190" spans="1:30" ht="12.75" hidden="1">
+    <row r="190" spans="1:30" ht="12.75">
       <c r="A190" s="4">
         <v>66286002346</v>
       </c>
@@ -24031,7 +24031,7 @@
       <c r="AC190" s="3"/>
       <c r="AD190" s="3"/>
     </row>
-    <row r="191" spans="1:30" ht="12.75" hidden="1">
+    <row r="191" spans="1:30" ht="12.75">
       <c r="A191" s="4">
         <v>41881109556</v>
       </c>
@@ -24109,7 +24109,7 @@
       <c r="AC191" s="3"/>
       <c r="AD191" s="3"/>
     </row>
-    <row r="192" spans="1:30" ht="12.75" hidden="1">
+    <row r="192" spans="1:30" ht="12.75">
       <c r="A192" s="4">
         <v>11481588536</v>
       </c>
@@ -24189,7 +24189,7 @@
       <c r="AC192" s="3"/>
       <c r="AD192" s="3"/>
     </row>
-    <row r="193" spans="1:30" ht="12.75" hidden="1">
+    <row r="193" spans="1:30" ht="12.75">
       <c r="A193" s="4">
         <v>21481994886</v>
       </c>
@@ -24269,7 +24269,7 @@
       <c r="AC193" s="3"/>
       <c r="AD193" s="3"/>
     </row>
-    <row r="194" spans="1:30" ht="12.75" hidden="1">
+    <row r="194" spans="1:30" ht="12.75">
       <c r="A194" s="4">
         <v>10986254146</v>
       </c>
@@ -24349,7 +24349,7 @@
       <c r="AC194" s="3"/>
       <c r="AD194" s="3"/>
     </row>
-    <row r="195" spans="1:30" ht="12.75" hidden="1">
+    <row r="195" spans="1:30" ht="12.75">
       <c r="A195" s="4">
         <v>10181162936</v>
       </c>
@@ -24429,7 +24429,7 @@
       <c r="AC195" s="3"/>
       <c r="AD195" s="3"/>
     </row>
-    <row r="196" spans="1:30" ht="12.75" hidden="1">
+    <row r="196" spans="1:30" ht="12.75">
       <c r="A196" s="4">
         <v>31281432696</v>
       </c>
@@ -24509,7 +24509,7 @@
       <c r="AC196" s="3"/>
       <c r="AD196" s="3"/>
     </row>
-    <row r="197" spans="1:30" ht="12.75" hidden="1">
+    <row r="197" spans="1:30" ht="12.75">
       <c r="A197" s="4">
         <v>20681354986</v>
       </c>
@@ -24587,7 +24587,7 @@
       <c r="AC197" s="3"/>
       <c r="AD197" s="3"/>
     </row>
-    <row r="198" spans="1:30" ht="12.75" hidden="1">
+    <row r="198" spans="1:30" ht="12.75">
       <c r="A198" s="4">
         <v>66286002346</v>
       </c>
@@ -24667,7 +24667,7 @@
       <c r="AC198" s="3"/>
       <c r="AD198" s="3"/>
     </row>
-    <row r="199" spans="1:30" ht="12.75" hidden="1">
+    <row r="199" spans="1:30" ht="12.75">
       <c r="A199" s="4">
         <v>60481181796</v>
       </c>
@@ -24747,7 +24747,7 @@
       <c r="AC199" s="3"/>
       <c r="AD199" s="3"/>
     </row>
-    <row r="200" spans="1:30" ht="12.75" hidden="1">
+    <row r="200" spans="1:30" ht="12.75">
       <c r="A200" s="4">
         <v>22081101166</v>
       </c>
@@ -24827,7 +24827,7 @@
       <c r="AC200" s="3"/>
       <c r="AD200" s="3"/>
     </row>
-    <row r="201" spans="1:30" ht="12.75" hidden="1">
+    <row r="201" spans="1:30" ht="12.75">
       <c r="A201" s="4">
         <v>14587001866</v>
       </c>
@@ -24903,7 +24903,7 @@
       <c r="AC201" s="3"/>
       <c r="AD201" s="3"/>
     </row>
-    <row r="202" spans="1:30" ht="12.75" hidden="1">
+    <row r="202" spans="1:30" ht="12.75">
       <c r="A202" s="4">
         <v>10781171936</v>
       </c>
@@ -24979,7 +24979,7 @@
       <c r="AC202" s="3"/>
       <c r="AD202" s="3"/>
     </row>
-    <row r="203" spans="1:30" ht="12.75" hidden="1">
+    <row r="203" spans="1:30" ht="12.75">
       <c r="A203" s="4">
         <v>90708487507</v>
       </c>
@@ -25055,7 +25055,7 @@
       <c r="AC203" s="3"/>
       <c r="AD203" s="3"/>
     </row>
-    <row r="204" spans="1:30" ht="12.75" hidden="1">
+    <row r="204" spans="1:30" ht="12.75">
       <c r="A204" s="4">
         <v>89286008546</v>
       </c>
@@ -25131,7 +25131,7 @@
       <c r="AC204" s="3"/>
       <c r="AD204" s="3"/>
     </row>
-    <row r="205" spans="1:30" ht="12.75" hidden="1">
+    <row r="205" spans="1:30" ht="12.75">
       <c r="A205" s="4">
         <v>60381255996</v>
       </c>
@@ -25207,7 +25207,7 @@
       <c r="AC205" s="3"/>
       <c r="AD205" s="3"/>
     </row>
-    <row r="206" spans="1:30" ht="12.75" hidden="1">
+    <row r="206" spans="1:30" ht="12.75">
       <c r="A206" s="4">
         <v>21188017576</v>
       </c>
@@ -25283,7 +25283,7 @@
       <c r="AC206" s="3"/>
       <c r="AD206" s="3"/>
     </row>
-    <row r="207" spans="1:30" ht="12.75" hidden="1">
+    <row r="207" spans="1:30" ht="12.75">
       <c r="A207" s="4">
         <v>21186195016</v>
       </c>
@@ -25359,7 +25359,7 @@
       <c r="AC207" s="3"/>
       <c r="AD207" s="3"/>
     </row>
-    <row r="208" spans="1:30" ht="12.75" hidden="1">
+    <row r="208" spans="1:30" ht="12.75">
       <c r="A208" s="4">
         <v>40981084366</v>
       </c>
@@ -25435,7 +25435,7 @@
       <c r="AC208" s="3"/>
       <c r="AD208" s="3"/>
     </row>
-    <row r="209" spans="1:30" ht="12.75" hidden="1">
+    <row r="209" spans="1:30" ht="12.75">
       <c r="A209" s="4">
         <v>21481699656</v>
       </c>
@@ -25511,7 +25511,7 @@
       <c r="AC209" s="3"/>
       <c r="AD209" s="3"/>
     </row>
-    <row r="210" spans="1:30" ht="12.75" hidden="1">
+    <row r="210" spans="1:30" ht="12.75">
       <c r="A210" s="4">
         <v>50681022806</v>
       </c>
@@ -25587,7 +25587,7 @@
       <c r="AC210" s="3"/>
       <c r="AD210" s="3"/>
     </row>
-    <row r="211" spans="1:30" ht="12.75" hidden="1">
+    <row r="211" spans="1:30" ht="12.75">
       <c r="A211" s="4">
         <v>10586667476</v>
       </c>
@@ -25661,7 +25661,7 @@
       <c r="AC211" s="3"/>
       <c r="AD211" s="3"/>
     </row>
-    <row r="212" spans="1:30" ht="12.75" hidden="1">
+    <row r="212" spans="1:30" ht="12.75">
       <c r="A212" s="4">
         <v>13486592786</v>
       </c>
@@ -25737,7 +25737,7 @@
       <c r="AC212" s="3"/>
       <c r="AD212" s="3"/>
     </row>
-    <row r="213" spans="1:30" ht="12.75" hidden="1">
+    <row r="213" spans="1:30" ht="12.75">
       <c r="A213" s="4">
         <v>22181003246</v>
       </c>
@@ -25813,7 +25813,7 @@
       <c r="AC213" s="3"/>
       <c r="AD213" s="3"/>
     </row>
-    <row r="214" spans="1:30" ht="12.75" hidden="1">
+    <row r="214" spans="1:30" ht="12.75">
       <c r="A214" s="4">
         <v>22681287446</v>
       </c>
@@ -25889,7 +25889,7 @@
       <c r="AC214" s="3"/>
       <c r="AD214" s="3"/>
     </row>
-    <row r="215" spans="1:30" ht="12.75" hidden="1">
+    <row r="215" spans="1:30" ht="12.75">
       <c r="A215" s="4">
         <v>50681022806</v>
       </c>
@@ -25965,7 +25965,7 @@
       <c r="AC215" s="3"/>
       <c r="AD215" s="3"/>
     </row>
-    <row r="216" spans="1:30" ht="12.75" hidden="1">
+    <row r="216" spans="1:30" ht="12.75">
       <c r="A216" s="4">
         <v>18686007116</v>
       </c>
@@ -26041,7 +26041,7 @@
       <c r="AC216" s="3"/>
       <c r="AD216" s="3"/>
     </row>
-    <row r="217" spans="1:30" ht="12.75" hidden="1">
+    <row r="217" spans="1:30" ht="12.75">
       <c r="A217" s="4">
         <v>10481181216</v>
       </c>
@@ -26117,7 +26117,7 @@
       <c r="AC217" s="3"/>
       <c r="AD217" s="3"/>
     </row>
-    <row r="218" spans="1:30" ht="12.75" hidden="1">
+    <row r="218" spans="1:30" ht="12.75">
       <c r="A218" s="4">
         <v>13786477096</v>
       </c>
@@ -26193,7 +26193,7 @@
       <c r="AC218" s="3"/>
       <c r="AD218" s="3"/>
     </row>
-    <row r="219" spans="1:30" ht="12.75" hidden="1">
+    <row r="219" spans="1:30" ht="12.75">
       <c r="A219" s="4">
         <v>13081763106</v>
       </c>
@@ -26269,7 +26269,7 @@
       <c r="AC219" s="3"/>
       <c r="AD219" s="3"/>
     </row>
-    <row r="220" spans="1:30" ht="12.75" hidden="1">
+    <row r="220" spans="1:30" ht="12.75">
       <c r="A220" s="4">
         <v>51787005336</v>
       </c>
@@ -26345,7 +26345,7 @@
       <c r="AC220" s="3"/>
       <c r="AD220" s="3"/>
     </row>
-    <row r="221" spans="1:30" ht="12.75" hidden="1">
+    <row r="221" spans="1:30" ht="12.75">
       <c r="A221" s="4">
         <v>31281096556</v>
       </c>
@@ -26419,7 +26419,7 @@
       <c r="AC221" s="3"/>
       <c r="AD221" s="3"/>
     </row>
-    <row r="222" spans="1:30" ht="12.75" hidden="1">
+    <row r="222" spans="1:30" ht="12.75">
       <c r="A222" s="4">
         <v>68181008706</v>
       </c>
@@ -26495,7 +26495,7 @@
       <c r="AC222" s="3"/>
       <c r="AD222" s="3"/>
     </row>
-    <row r="223" spans="1:30" ht="12.75" hidden="1">
+    <row r="223" spans="1:30" ht="12.75">
       <c r="A223" s="4">
         <v>11681061766</v>
       </c>
@@ -26571,7 +26571,7 @@
       <c r="AC223" s="3"/>
       <c r="AD223" s="3"/>
     </row>
-    <row r="224" spans="1:30" ht="12.75" hidden="1">
+    <row r="224" spans="1:30" ht="12.75">
       <c r="A224" s="4">
         <v>10181162936</v>
       </c>
@@ -26647,7 +26647,7 @@
       <c r="AC224" s="3"/>
       <c r="AD224" s="3"/>
     </row>
-    <row r="225" spans="1:30" ht="12.75" hidden="1">
+    <row r="225" spans="1:30" ht="12.75">
       <c r="A225" s="4">
         <v>60781372536</v>
       </c>
@@ -26723,7 +26723,7 @@
       <c r="AC225" s="3"/>
       <c r="AD225" s="3"/>
     </row>
-    <row r="226" spans="1:30" ht="12.75" hidden="1">
+    <row r="226" spans="1:30" ht="12.75">
       <c r="A226" s="4">
         <v>11781094056</v>
       </c>
@@ -26799,7 +26799,7 @@
       <c r="AC226" s="3"/>
       <c r="AD226" s="3"/>
     </row>
-    <row r="227" spans="1:30" ht="12.75" hidden="1">
+    <row r="227" spans="1:30" ht="12.75">
       <c r="A227" s="4">
         <v>20681568726</v>
       </c>
@@ -26875,7 +26875,7 @@
       <c r="AC227" s="3"/>
       <c r="AD227" s="3"/>
     </row>
-    <row r="228" spans="1:30" ht="12.75" hidden="1">
+    <row r="228" spans="1:30" ht="12.75">
       <c r="A228" s="4">
         <v>91204354277</v>
       </c>
@@ -26951,7 +26951,7 @@
       <c r="AC228" s="3"/>
       <c r="AD228" s="3"/>
     </row>
-    <row r="229" spans="1:30" ht="12.75" hidden="1">
+    <row r="229" spans="1:30" ht="12.75">
       <c r="A229" s="4">
         <v>10181162936</v>
       </c>
@@ -27027,7 +27027,7 @@
       <c r="AC229" s="3"/>
       <c r="AD229" s="3"/>
     </row>
-    <row r="230" spans="1:30" ht="12.75" hidden="1">
+    <row r="230" spans="1:30" ht="12.75">
       <c r="A230" s="4">
         <v>30881052856</v>
       </c>
@@ -27103,7 +27103,7 @@
       <c r="AC230" s="3"/>
       <c r="AD230" s="3"/>
     </row>
-    <row r="231" spans="1:30" ht="12.75" hidden="1">
+    <row r="231" spans="1:30" ht="12.75">
       <c r="A231" s="4">
         <v>41181210296</v>
       </c>
@@ -27179,7 +27179,7 @@
       <c r="AC231" s="3"/>
       <c r="AD231" s="3"/>
     </row>
-    <row r="232" spans="1:30" ht="12.75" hidden="1">
+    <row r="232" spans="1:30" ht="12.75">
       <c r="A232" s="4">
         <v>33886004196</v>
       </c>
@@ -27255,7 +27255,7 @@
       <c r="AC232" s="3"/>
       <c r="AD232" s="3"/>
     </row>
-    <row r="233" spans="1:30" ht="12.75" hidden="1">
+    <row r="233" spans="1:30" ht="12.75">
       <c r="A233" s="4">
         <v>33886004196</v>
       </c>
@@ -27331,7 +27331,7 @@
       <c r="AC233" s="3"/>
       <c r="AD233" s="3"/>
     </row>
-    <row r="234" spans="1:30" ht="12.75" hidden="1">
+    <row r="234" spans="1:30" ht="12.75">
       <c r="A234" s="4">
         <v>10181667556</v>
       </c>
@@ -27407,7 +27407,7 @@
       <c r="AC234" s="3"/>
       <c r="AD234" s="3"/>
     </row>
-    <row r="235" spans="1:30" ht="12.75" hidden="1">
+    <row r="235" spans="1:30" ht="12.75">
       <c r="A235" s="4">
         <v>10481181216</v>
       </c>
@@ -27483,7 +27483,7 @@
       <c r="AC235" s="3"/>
       <c r="AD235" s="3"/>
     </row>
-    <row r="236" spans="1:30" ht="12.75" hidden="1">
+    <row r="236" spans="1:30" ht="12.75">
       <c r="A236" s="4">
         <v>86887003676</v>
       </c>
@@ -27559,7 +27559,7 @@
       <c r="AC236" s="3"/>
       <c r="AD236" s="3"/>
     </row>
-    <row r="237" spans="1:30" ht="12.75" hidden="1">
+    <row r="237" spans="1:30" ht="12.75">
       <c r="A237" s="4">
         <v>11481046056</v>
       </c>
@@ -27635,7 +27635,7 @@
       <c r="AC237" s="3"/>
       <c r="AD237" s="3"/>
     </row>
-    <row r="238" spans="1:30" ht="12.75" hidden="1">
+    <row r="238" spans="1:30" ht="12.75">
       <c r="A238" s="4">
         <v>30881052856</v>
       </c>
@@ -27711,7 +27711,7 @@
       <c r="AC238" s="3"/>
       <c r="AD238" s="3"/>
     </row>
-    <row r="239" spans="1:30" ht="12.75" hidden="1">
+    <row r="239" spans="1:30" ht="12.75">
       <c r="A239" s="4">
         <v>90904945447</v>
       </c>
@@ -27787,7 +27787,7 @@
       <c r="AC239" s="3"/>
       <c r="AD239" s="3"/>
     </row>
-    <row r="240" spans="1:30" ht="12.75" hidden="1">
+    <row r="240" spans="1:30" ht="12.75">
       <c r="A240" s="4">
         <v>40381132706</v>
       </c>
@@ -27863,7 +27863,7 @@
       <c r="AC240" s="3"/>
       <c r="AD240" s="3"/>
     </row>
-    <row r="241" spans="1:30" ht="12.75" hidden="1">
+    <row r="241" spans="1:30" ht="12.75">
       <c r="A241" s="4">
         <v>40281173656</v>
       </c>
@@ -27939,7 +27939,7 @@
       <c r="AC241" s="3"/>
       <c r="AD241" s="3"/>
     </row>
-    <row r="242" spans="1:30" ht="12.75" hidden="1">
+    <row r="242" spans="1:30" ht="12.75">
       <c r="A242" s="4">
         <v>13681120516</v>
       </c>
@@ -28015,7 +28015,7 @@
       <c r="AC242" s="3"/>
       <c r="AD242" s="3"/>
     </row>
-    <row r="243" spans="1:30" ht="12.75" hidden="1">
+    <row r="243" spans="1:30" ht="12.75">
       <c r="A243" s="4">
         <v>41781128486</v>
       </c>
@@ -28091,7 +28091,7 @@
       <c r="AC243" s="3"/>
       <c r="AD243" s="3"/>
     </row>
-    <row r="244" spans="1:30" ht="12.75" hidden="1">
+    <row r="244" spans="1:30" ht="12.75">
       <c r="A244" s="4">
         <v>50281628216</v>
       </c>
@@ -28167,7 +28167,7 @@
       <c r="AC244" s="3"/>
       <c r="AD244" s="3"/>
     </row>
-    <row r="245" spans="1:30" ht="12.75" hidden="1">
+    <row r="245" spans="1:30" ht="12.75">
       <c r="A245" s="4">
         <v>10181349286</v>
       </c>
@@ -28243,7 +28243,7 @@
       <c r="AC245" s="3"/>
       <c r="AD245" s="3"/>
     </row>
-    <row r="246" spans="1:30" ht="12.75" hidden="1">
+    <row r="246" spans="1:30" ht="12.75">
       <c r="A246" s="4">
         <v>30881052856</v>
       </c>
@@ -28319,7 +28319,7 @@
       <c r="AC246" s="3"/>
       <c r="AD246" s="3"/>
     </row>
-    <row r="247" spans="1:30" ht="12.75" hidden="1">
+    <row r="247" spans="1:30" ht="12.75">
       <c r="A247" s="4">
         <v>20981104776</v>
       </c>
@@ -28395,7 +28395,7 @@
       <c r="AC247" s="3"/>
       <c r="AD247" s="3"/>
     </row>
-    <row r="248" spans="1:30" ht="12.75" hidden="1">
+    <row r="248" spans="1:30" ht="12.75">
       <c r="A248" s="4">
         <v>60581991226</v>
       </c>
@@ -28471,7 +28471,7 @@
       <c r="AC248" s="3"/>
       <c r="AD248" s="3"/>
     </row>
-    <row r="249" spans="1:30" ht="12.75" hidden="1">
+    <row r="249" spans="1:30" ht="12.75">
       <c r="A249" s="4">
         <v>12286052216</v>
       </c>
@@ -28547,7 +28547,7 @@
       <c r="AC249" s="3"/>
       <c r="AD249" s="3"/>
     </row>
-    <row r="250" spans="1:30" ht="12.75" hidden="1">
+    <row r="250" spans="1:30" ht="12.75">
       <c r="A250" s="4">
         <v>41681133686</v>
       </c>
@@ -28623,7 +28623,7 @@
       <c r="AC250" s="3"/>
       <c r="AD250" s="3"/>
     </row>
-    <row r="251" spans="1:30" ht="12.75" hidden="1">
+    <row r="251" spans="1:30" ht="12.75">
       <c r="A251" s="4">
         <v>31281191486</v>
       </c>
@@ -28699,7 +28699,7 @@
       <c r="AC251" s="3"/>
       <c r="AD251" s="3"/>
     </row>
-    <row r="252" spans="1:30" ht="12.75" hidden="1">
+    <row r="252" spans="1:30" ht="12.75">
       <c r="A252" s="4">
         <v>22681287446</v>
       </c>
@@ -28775,7 +28775,7 @@
       <c r="AC252" s="3"/>
       <c r="AD252" s="3"/>
     </row>
-    <row r="253" spans="1:30" ht="12.75" hidden="1">
+    <row r="253" spans="1:30" ht="12.75">
       <c r="A253" s="4">
         <v>24588002756</v>
       </c>
@@ -28851,7 +28851,7 @@
       <c r="AC253" s="3"/>
       <c r="AD253" s="3"/>
     </row>
-    <row r="254" spans="1:30" ht="12.75" hidden="1">
+    <row r="254" spans="1:30" ht="12.75">
       <c r="A254" s="4">
         <v>90700104187</v>
       </c>
@@ -28927,7 +28927,7 @@
       <c r="AC254" s="3"/>
       <c r="AD254" s="3"/>
     </row>
-    <row r="255" spans="1:30" ht="12.75" hidden="1">
+    <row r="255" spans="1:30" ht="12.75">
       <c r="A255" s="4">
         <v>62181431786</v>
       </c>
@@ -29003,7 +29003,7 @@
       <c r="AC255" s="3"/>
       <c r="AD255" s="3"/>
     </row>
-    <row r="256" spans="1:30" ht="12.75" hidden="1">
+    <row r="256" spans="1:30" ht="12.75">
       <c r="A256" s="4">
         <v>43081005166</v>
       </c>
@@ -29079,7 +29079,7 @@
       <c r="AC256" s="3"/>
       <c r="AD256" s="3"/>
     </row>
-    <row r="257" spans="1:30" ht="12.75" hidden="1">
+    <row r="257" spans="1:30" ht="12.75">
       <c r="A257" s="4">
         <v>22086088386</v>
       </c>
@@ -29155,7 +29155,7 @@
       <c r="AC257" s="3"/>
       <c r="AD257" s="3"/>
     </row>
-    <row r="258" spans="1:30" ht="12.75" hidden="1">
+    <row r="258" spans="1:30" ht="12.75">
       <c r="A258" s="4">
         <v>14081004766</v>
       </c>
@@ -29231,7 +29231,7 @@
       <c r="AC258" s="3"/>
       <c r="AD258" s="3"/>
     </row>
-    <row r="259" spans="1:30" ht="12.75" hidden="1">
+    <row r="259" spans="1:30" ht="12.75">
       <c r="A259" s="4">
         <v>22086088386</v>
       </c>
@@ -29307,7 +29307,7 @@
       <c r="AC259" s="3"/>
       <c r="AD259" s="3"/>
     </row>
-    <row r="260" spans="1:30" ht="12.75" hidden="1">
+    <row r="260" spans="1:30" ht="12.75">
       <c r="A260" s="4">
         <v>25881001416</v>
       </c>
@@ -29383,7 +29383,7 @@
       <c r="AC260" s="3"/>
       <c r="AD260" s="3"/>
     </row>
-    <row r="261" spans="1:30" ht="12.75" hidden="1">
+    <row r="261" spans="1:30" ht="12.75">
       <c r="A261" s="4">
         <v>40881452346</v>
       </c>
@@ -29459,7 +29459,7 @@
       <c r="AC261" s="3"/>
       <c r="AD261" s="3"/>
     </row>
-    <row r="262" spans="1:30" ht="12.75" hidden="1">
+    <row r="262" spans="1:30" ht="12.75">
       <c r="A262" s="4">
         <v>13681120516</v>
       </c>
@@ -29535,7 +29535,7 @@
       <c r="AC262" s="3"/>
       <c r="AD262" s="3"/>
     </row>
-    <row r="263" spans="1:30" ht="12.75" hidden="1">
+    <row r="263" spans="1:30" ht="12.75">
       <c r="A263" s="4">
         <v>10181162936</v>
       </c>
@@ -29609,7 +29609,7 @@
       <c r="AC263" s="3"/>
       <c r="AD263" s="3"/>
     </row>
-    <row r="264" spans="1:30" ht="12.75" hidden="1">
+    <row r="264" spans="1:30" ht="12.75">
       <c r="A264" s="4">
         <v>11481163776</v>
       </c>
@@ -29685,7 +29685,7 @@
       <c r="AC264" s="3"/>
       <c r="AD264" s="3"/>
     </row>
-    <row r="265" spans="1:30" ht="12.75" hidden="1">
+    <row r="265" spans="1:30" ht="12.75">
       <c r="A265" s="4">
         <v>50381543586</v>
       </c>
@@ -29761,7 +29761,7 @@
       <c r="AC265" s="3"/>
       <c r="AD265" s="3"/>
     </row>
-    <row r="266" spans="1:30" ht="12.75" hidden="1">
+    <row r="266" spans="1:30" ht="12.75">
       <c r="A266" s="4">
         <v>90700104187</v>
       </c>
@@ -29837,7 +29837,7 @@
       <c r="AC266" s="3"/>
       <c r="AD266" s="3"/>
     </row>
-    <row r="267" spans="1:30" ht="12.75" hidden="1">
+    <row r="267" spans="1:30" ht="12.75">
       <c r="A267" s="4">
         <v>12081528016</v>
       </c>
@@ -29913,7 +29913,7 @@
       <c r="AC267" s="3"/>
       <c r="AD267" s="3"/>
     </row>
-    <row r="268" spans="1:30" ht="12.75" hidden="1">
+    <row r="268" spans="1:30" ht="12.75">
       <c r="A268" s="4">
         <v>11981361026</v>
       </c>
@@ -29989,7 +29989,7 @@
       <c r="AC268" s="3"/>
       <c r="AD268" s="3"/>
     </row>
-    <row r="269" spans="1:30" ht="12.75" hidden="1">
+    <row r="269" spans="1:30" ht="12.75">
       <c r="A269" s="4">
         <v>10581595196</v>
       </c>
@@ -30065,7 +30065,7 @@
       <c r="AC269" s="3"/>
       <c r="AD269" s="3"/>
     </row>
-    <row r="270" spans="1:30" ht="12.75" hidden="1">
+    <row r="270" spans="1:30" ht="12.75">
       <c r="A270" s="4">
         <v>60881045516</v>
       </c>
@@ -30141,7 +30141,7 @@
       <c r="AC270" s="3"/>
       <c r="AD270" s="3"/>
     </row>
-    <row r="271" spans="1:30" ht="12.75" hidden="1">
+    <row r="271" spans="1:30" ht="12.75">
       <c r="A271" s="4">
         <v>10481181216</v>
       </c>
@@ -30217,7 +30217,7 @@
       <c r="AC271" s="3"/>
       <c r="AD271" s="3"/>
     </row>
-    <row r="272" spans="1:30" ht="12.75" hidden="1">
+    <row r="272" spans="1:30" ht="12.75">
       <c r="A272" s="4">
         <v>11481588536</v>
       </c>
@@ -30293,7 +30293,7 @@
       <c r="AC272" s="3"/>
       <c r="AD272" s="3"/>
     </row>
-    <row r="273" spans="1:30" ht="12.75" hidden="1">
+    <row r="273" spans="1:30" ht="12.75">
       <c r="A273" s="4">
         <v>10481181216</v>
       </c>
@@ -30369,7 +30369,7 @@
       <c r="AC273" s="3"/>
       <c r="AD273" s="3"/>
     </row>
-    <row r="274" spans="1:30" ht="12.75" hidden="1">
+    <row r="274" spans="1:30" ht="12.75">
       <c r="A274" s="4">
         <v>10481181216</v>
       </c>
@@ -30445,7 +30445,7 @@
       <c r="AC274" s="3"/>
       <c r="AD274" s="3"/>
     </row>
-    <row r="275" spans="1:30" ht="12.75" hidden="1">
+    <row r="275" spans="1:30" ht="12.75">
       <c r="A275" s="4">
         <v>22081040506</v>
       </c>
@@ -30521,7 +30521,7 @@
       <c r="AC275" s="3"/>
       <c r="AD275" s="3"/>
     </row>
-    <row r="276" spans="1:30" ht="12.75" hidden="1">
+    <row r="276" spans="1:30" ht="12.75">
       <c r="A276" s="4">
         <v>13381227356</v>
       </c>
@@ -30597,7 +30597,7 @@
       <c r="AC276" s="3"/>
       <c r="AD276" s="3"/>
     </row>
-    <row r="277" spans="1:30" ht="12.75" hidden="1">
+    <row r="277" spans="1:30" ht="12.75">
       <c r="A277" s="4">
         <v>41681133686</v>
       </c>
@@ -30673,7 +30673,7 @@
       <c r="AC277" s="3"/>
       <c r="AD277" s="3"/>
     </row>
-    <row r="278" spans="1:30" ht="12.75" hidden="1">
+    <row r="278" spans="1:30" ht="12.75">
       <c r="A278" s="4">
         <v>90700104187</v>
       </c>
@@ -30749,7 +30749,7 @@
       <c r="AC278" s="3"/>
       <c r="AD278" s="3"/>
     </row>
-    <row r="279" spans="1:30" ht="12.75" hidden="1">
+    <row r="279" spans="1:30" ht="12.75">
       <c r="A279" s="4">
         <v>31286189746</v>
       </c>
@@ -30901,7 +30901,7 @@
       <c r="AC280" s="3"/>
       <c r="AD280" s="3"/>
     </row>
-    <row r="281" spans="1:30" ht="12.75" hidden="1">
+    <row r="281" spans="1:30" ht="12.75">
       <c r="A281" s="4">
         <v>35581012146</v>
       </c>
@@ -30977,7 +30977,7 @@
       <c r="AC281" s="3"/>
       <c r="AD281" s="3"/>
     </row>
-    <row r="282" spans="1:30" ht="12.75" hidden="1">
+    <row r="282" spans="1:30" ht="12.75">
       <c r="A282" s="4">
         <v>31481079546</v>
       </c>
@@ -31053,7 +31053,7 @@
       <c r="AC282" s="3"/>
       <c r="AD282" s="3"/>
     </row>
-    <row r="283" spans="1:30" ht="12.75" hidden="1">
+    <row r="283" spans="1:30" ht="12.75">
       <c r="A283" s="4">
         <v>90700104187</v>
       </c>
@@ -31129,7 +31129,7 @@
       <c r="AC283" s="3"/>
       <c r="AD283" s="3"/>
     </row>
-    <row r="284" spans="1:30" ht="12.75" hidden="1">
+    <row r="284" spans="1:30" ht="12.75">
       <c r="A284" s="4">
         <v>40981741066</v>
       </c>
@@ -31205,7 +31205,7 @@
       <c r="AC284" s="3"/>
       <c r="AD284" s="3"/>
     </row>
-    <row r="285" spans="1:30" ht="12.75" hidden="1">
+    <row r="285" spans="1:30" ht="12.75">
       <c r="A285" s="4">
         <v>21487991226</v>
       </c>
@@ -31281,7 +31281,7 @@
       <c r="AC285" s="3"/>
       <c r="AD285" s="3"/>
     </row>
-    <row r="286" spans="1:30" ht="12.75" hidden="1">
+    <row r="286" spans="1:30" ht="12.75">
       <c r="A286" s="4">
         <v>12781611126</v>
       </c>
@@ -31357,7 +31357,7 @@
       <c r="AC286" s="3"/>
       <c r="AD286" s="3"/>
     </row>
-    <row r="287" spans="1:30" ht="12.75" hidden="1">
+    <row r="287" spans="1:30" ht="12.75">
       <c r="A287" s="4">
         <v>12487160946</v>
       </c>
@@ -31433,7 +31433,7 @@
       <c r="AC287" s="3"/>
       <c r="AD287" s="3"/>
     </row>
-    <row r="288" spans="1:30" ht="12.75" hidden="1">
+    <row r="288" spans="1:30" ht="12.75">
       <c r="A288" s="4">
         <v>31481079546</v>
       </c>
@@ -31509,7 +31509,7 @@
       <c r="AC288" s="3"/>
       <c r="AD288" s="3"/>
     </row>
-    <row r="289" spans="1:30" ht="12.75" hidden="1">
+    <row r="289" spans="1:30" ht="12.75">
       <c r="A289" s="4">
         <v>13981098416</v>
       </c>
@@ -31585,7 +31585,7 @@
       <c r="AC289" s="3"/>
       <c r="AD289" s="3"/>
     </row>
-    <row r="290" spans="1:30" ht="12.75" hidden="1">
+    <row r="290" spans="1:30" ht="12.75">
       <c r="A290" s="4">
         <v>60781330676</v>
       </c>
@@ -31661,7 +31661,7 @@
       <c r="AC290" s="3"/>
       <c r="AD290" s="3"/>
     </row>
-    <row r="291" spans="1:30" ht="12.75" hidden="1">
+    <row r="291" spans="1:30" ht="12.75">
       <c r="A291" s="4">
         <v>51481828686</v>
       </c>
@@ -31737,7 +31737,7 @@
       <c r="AC291" s="3"/>
       <c r="AD291" s="3"/>
     </row>
-    <row r="292" spans="1:30" ht="12.75" hidden="1">
+    <row r="292" spans="1:30" ht="12.75">
       <c r="A292" s="4">
         <v>10581296406</v>
       </c>
@@ -31813,7 +31813,7 @@
       <c r="AC292" s="3"/>
       <c r="AD292" s="3"/>
     </row>
-    <row r="293" spans="1:30" ht="12.75" hidden="1">
+    <row r="293" spans="1:30" ht="12.75">
       <c r="A293" s="4">
         <v>18381002986</v>
       </c>
@@ -31889,7 +31889,7 @@
       <c r="AC293" s="3"/>
       <c r="AD293" s="3"/>
     </row>
-    <row r="294" spans="1:30" ht="12.75" hidden="1">
+    <row r="294" spans="1:30" ht="12.75">
       <c r="A294" s="4">
         <v>22087461116</v>
       </c>
@@ -31965,7 +31965,7 @@
       <c r="AC294" s="3"/>
       <c r="AD294" s="3"/>
     </row>
-    <row r="295" spans="1:30" ht="12.75" hidden="1">
+    <row r="295" spans="1:30" ht="12.75">
       <c r="A295" s="4">
         <v>12481705156</v>
       </c>
@@ -32041,7 +32041,7 @@
       <c r="AC295" s="3"/>
       <c r="AD295" s="3"/>
     </row>
-    <row r="296" spans="1:30" ht="12.75" hidden="1">
+    <row r="296" spans="1:30" ht="12.75">
       <c r="A296" s="4">
         <v>40881215286</v>
       </c>
@@ -32117,7 +32117,7 @@
       <c r="AC296" s="3"/>
       <c r="AD296" s="3"/>
     </row>
-    <row r="297" spans="1:30" ht="12.75" hidden="1">
+    <row r="297" spans="1:30" ht="12.75">
       <c r="A297" s="4">
         <v>60981485906</v>
       </c>
@@ -32193,7 +32193,7 @@
       <c r="AC297" s="3"/>
       <c r="AD297" s="3"/>
     </row>
-    <row r="298" spans="1:30" ht="12.75" hidden="1">
+    <row r="298" spans="1:30" ht="12.75">
       <c r="A298" s="4">
         <v>90700104187</v>
       </c>
@@ -32269,7 +32269,7 @@
       <c r="AC298" s="3"/>
       <c r="AD298" s="3"/>
     </row>
-    <row r="299" spans="1:30" ht="12.75" hidden="1">
+    <row r="299" spans="1:30" ht="12.75">
       <c r="A299" s="4">
         <v>10681327696</v>
       </c>
@@ -32345,7 +32345,7 @@
       <c r="AC299" s="3"/>
       <c r="AD299" s="3"/>
     </row>
-    <row r="300" spans="1:30" ht="12.75" hidden="1">
+    <row r="300" spans="1:30" ht="12.75">
       <c r="A300" s="4">
         <v>12286060836</v>
       </c>
@@ -32421,7 +32421,7 @@
       <c r="AC300" s="3"/>
       <c r="AD300" s="3"/>
     </row>
-    <row r="301" spans="1:30" ht="12.75" hidden="1">
+    <row r="301" spans="1:30" ht="12.75">
       <c r="A301" s="4">
         <v>31481966136</v>
       </c>
@@ -32501,7 +32501,7 @@
       <c r="AC301" s="3"/>
       <c r="AD301" s="3"/>
     </row>
-    <row r="302" spans="1:30" ht="12.75" hidden="1">
+    <row r="302" spans="1:30" ht="12.75">
       <c r="A302" s="4">
         <v>41086447236</v>
       </c>
@@ -32581,7 +32581,7 @@
       <c r="AC302" s="3"/>
       <c r="AD302" s="3"/>
     </row>
-    <row r="303" spans="1:30" ht="12.75" hidden="1">
+    <row r="303" spans="1:30" ht="12.75">
       <c r="A303" s="4">
         <v>90702173657</v>
       </c>
@@ -32661,7 +32661,7 @@
       <c r="AC303" s="3"/>
       <c r="AD303" s="3"/>
     </row>
-    <row r="304" spans="1:30" ht="12.75" hidden="1">
+    <row r="304" spans="1:30" ht="12.75">
       <c r="A304" s="4">
         <v>41481026426</v>
       </c>
@@ -32741,7 +32741,7 @@
       <c r="AC304" s="3"/>
       <c r="AD304" s="3"/>
     </row>
-    <row r="305" spans="1:30" ht="12.75" hidden="1">
+    <row r="305" spans="1:30" ht="12.75">
       <c r="A305" s="4">
         <v>10181667556</v>
       </c>
@@ -32821,7 +32821,7 @@
       <c r="AC305" s="3"/>
       <c r="AD305" s="3"/>
     </row>
-    <row r="306" spans="1:30" ht="12.75" hidden="1">
+    <row r="306" spans="1:30" ht="12.75">
       <c r="A306" s="4">
         <v>22081193306</v>
       </c>
@@ -32901,7 +32901,7 @@
       <c r="AC306" s="3"/>
       <c r="AD306" s="3"/>
     </row>
-    <row r="307" spans="1:30" ht="12.75" hidden="1">
+    <row r="307" spans="1:30" ht="12.75">
       <c r="A307" s="4">
         <v>60181141556</v>
       </c>
@@ -32981,7 +32981,7 @@
       <c r="AC307" s="3"/>
       <c r="AD307" s="3"/>
     </row>
-    <row r="308" spans="1:30" ht="12.75" hidden="1">
+    <row r="308" spans="1:30" ht="12.75">
       <c r="A308" s="4">
         <v>40981084366</v>
       </c>
@@ -33061,7 +33061,7 @@
       <c r="AC308" s="3"/>
       <c r="AD308" s="3"/>
     </row>
-    <row r="309" spans="1:30" ht="12.75" hidden="1">
+    <row r="309" spans="1:30" ht="12.75">
       <c r="A309" s="4">
         <v>22081193306</v>
       </c>
@@ -33141,7 +33141,7 @@
       <c r="AC309" s="3"/>
       <c r="AD309" s="3"/>
     </row>
-    <row r="310" spans="1:30" ht="12.75" hidden="1">
+    <row r="310" spans="1:30" ht="12.75">
       <c r="A310" s="4">
         <v>10881659136</v>
       </c>
@@ -33219,7 +33219,7 @@
       <c r="AC310" s="3"/>
       <c r="AD310" s="3"/>
     </row>
-    <row r="311" spans="1:30" ht="12.75" hidden="1">
+    <row r="311" spans="1:30" ht="12.75">
       <c r="A311" s="4">
         <v>40986014386</v>
       </c>
@@ -33299,7 +33299,7 @@
       <c r="AC311" s="3"/>
       <c r="AD311" s="3"/>
     </row>
-    <row r="312" spans="1:30" ht="12.75" hidden="1">
+    <row r="312" spans="1:30" ht="12.75">
       <c r="A312" s="4">
         <v>20685237586</v>
       </c>
@@ -33379,7 +33379,7 @@
       <c r="AC312" s="3"/>
       <c r="AD312" s="3"/>
     </row>
-    <row r="313" spans="1:30" ht="12.75" hidden="1">
+    <row r="313" spans="1:30" ht="12.75">
       <c r="A313" s="4">
         <v>20181450836</v>
       </c>
@@ -33459,7 +33459,7 @@
       <c r="AC313" s="3"/>
       <c r="AD313" s="3"/>
     </row>
-    <row r="314" spans="1:30" ht="12.75" hidden="1">
+    <row r="314" spans="1:30" ht="12.75">
       <c r="A314" s="4">
         <v>90700104187</v>
       </c>
@@ -33539,7 +33539,7 @@
       <c r="AC314" s="3"/>
       <c r="AD314" s="3"/>
     </row>
-    <row r="315" spans="1:30" ht="12.75" hidden="1">
+    <row r="315" spans="1:30" ht="12.75">
       <c r="A315" s="4">
         <v>20281459756</v>
       </c>
@@ -33619,7 +33619,7 @@
       <c r="AC315" s="3"/>
       <c r="AD315" s="3"/>
     </row>
-    <row r="316" spans="1:30" ht="12.75" hidden="1">
+    <row r="316" spans="1:30" ht="12.75">
       <c r="A316" s="4">
         <v>22081993916</v>
       </c>
@@ -33699,7 +33699,7 @@
       <c r="AC316" s="3"/>
       <c r="AD316" s="3"/>
     </row>
-    <row r="317" spans="1:30" ht="12.75" hidden="1">
+    <row r="317" spans="1:30" ht="12.75">
       <c r="A317" s="4">
         <v>31281083406</v>
       </c>
@@ -33779,7 +33779,7 @@
       <c r="AC317" s="3"/>
       <c r="AD317" s="3"/>
     </row>
-    <row r="318" spans="1:30" ht="12.75" hidden="1">
+    <row r="318" spans="1:30" ht="12.75">
       <c r="A318" s="4">
         <v>22081993916</v>
       </c>
@@ -33859,7 +33859,7 @@
       <c r="AC318" s="3"/>
       <c r="AD318" s="3"/>
     </row>
-    <row r="319" spans="1:30" ht="12.75" hidden="1">
+    <row r="319" spans="1:30" ht="12.75">
       <c r="A319" s="4">
         <v>21188517286</v>
       </c>
@@ -33939,7 +33939,7 @@
       <c r="AC319" s="3"/>
       <c r="AD319" s="3"/>
     </row>
-    <row r="320" spans="1:30" ht="12.75" hidden="1">
+    <row r="320" spans="1:30" ht="12.75">
       <c r="A320" s="4">
         <v>41086447236</v>
       </c>
@@ -34019,7 +34019,7 @@
       <c r="AC320" s="3"/>
       <c r="AD320" s="3"/>
     </row>
-    <row r="321" spans="1:30" ht="12.75" hidden="1">
+    <row r="321" spans="1:30" ht="12.75">
       <c r="A321" s="4">
         <v>21481108396</v>
       </c>
@@ -34099,7 +34099,7 @@
       <c r="AC321" s="3"/>
       <c r="AD321" s="3"/>
     </row>
-    <row r="322" spans="1:30" ht="12.75" hidden="1">
+    <row r="322" spans="1:30" ht="12.75">
       <c r="A322" s="4">
         <v>40881202096</v>
       </c>
@@ -34179,7 +34179,7 @@
       <c r="AC322" s="3"/>
       <c r="AD322" s="3"/>
     </row>
-    <row r="323" spans="1:30" ht="12.75" hidden="1">
+    <row r="323" spans="1:30" ht="12.75">
       <c r="A323" s="4">
         <v>13181783446</v>
       </c>
@@ -34259,7 +34259,7 @@
       <c r="AC323" s="3"/>
       <c r="AD323" s="3"/>
     </row>
-    <row r="324" spans="1:30" ht="12.75" hidden="1">
+    <row r="324" spans="1:30" ht="12.75">
       <c r="A324" s="4">
         <v>13981126716</v>
       </c>
@@ -34339,7 +34339,7 @@
       <c r="AC324" s="3"/>
       <c r="AD324" s="3"/>
     </row>
-    <row r="325" spans="1:30" ht="12.75" hidden="1">
+    <row r="325" spans="1:30" ht="12.75">
       <c r="A325" s="4">
         <v>10181349286</v>
       </c>
@@ -34419,7 +34419,7 @@
       <c r="AC325" s="3"/>
       <c r="AD325" s="3"/>
     </row>
-    <row r="326" spans="1:30" ht="12.75" hidden="1">
+    <row r="326" spans="1:30" ht="12.75">
       <c r="A326" s="4">
         <v>31381028066</v>
       </c>
@@ -34499,7 +34499,7 @@
       <c r="AC326" s="3"/>
       <c r="AD326" s="3"/>
     </row>
-    <row r="327" spans="1:30" ht="12.75" hidden="1">
+    <row r="327" spans="1:30" ht="12.75">
       <c r="A327" s="4">
         <v>31481062896</v>
       </c>
@@ -34579,7 +34579,7 @@
       <c r="AC327" s="3"/>
       <c r="AD327" s="3"/>
     </row>
-    <row r="328" spans="1:30" ht="12.75" hidden="1">
+    <row r="328" spans="1:30" ht="12.75">
       <c r="A328" s="4">
         <v>21081583936</v>
       </c>
@@ -34659,7 +34659,7 @@
       <c r="AC328" s="3"/>
       <c r="AD328" s="3"/>
     </row>
-    <row r="329" spans="1:30" ht="12.75" hidden="1">
+    <row r="329" spans="1:30" ht="12.75">
       <c r="A329" s="4">
         <v>11081050346</v>
       </c>
@@ -34739,7 +34739,7 @@
       <c r="AC329" s="3"/>
       <c r="AD329" s="3"/>
     </row>
-    <row r="330" spans="1:30" ht="12.75" hidden="1">
+    <row r="330" spans="1:30" ht="12.75">
       <c r="A330" s="4">
         <v>23181016886</v>
       </c>
@@ -34819,7 +34819,7 @@
       <c r="AC330" s="3"/>
       <c r="AD330" s="3"/>
     </row>
-    <row r="331" spans="1:30" ht="12.75" hidden="1">
+    <row r="331" spans="1:30" ht="12.75">
       <c r="A331" s="4">
         <v>13581643146</v>
       </c>
@@ -34899,7 +34899,7 @@
       <c r="AC331" s="3"/>
       <c r="AD331" s="3"/>
     </row>
-    <row r="332" spans="1:30" ht="12.75" hidden="1">
+    <row r="332" spans="1:30" ht="12.75">
       <c r="A332" s="4">
         <v>10181349286</v>
       </c>
@@ -34979,7 +34979,7 @@
       <c r="AC332" s="3"/>
       <c r="AD332" s="3"/>
     </row>
-    <row r="333" spans="1:30" ht="12.75" hidden="1">
+    <row r="333" spans="1:30" ht="12.75">
       <c r="A333" s="4">
         <v>90700104187</v>
       </c>
@@ -35059,7 +35059,7 @@
       <c r="AC333" s="3"/>
       <c r="AD333" s="3"/>
     </row>
-    <row r="334" spans="1:30" ht="12.75" hidden="1">
+    <row r="334" spans="1:30" ht="12.75">
       <c r="A334" s="4">
         <v>11481163776</v>
       </c>
@@ -35139,7 +35139,7 @@
       <c r="AC334" s="3"/>
       <c r="AD334" s="3"/>
     </row>
-    <row r="335" spans="1:30" ht="12.75" hidden="1">
+    <row r="335" spans="1:30" ht="12.75">
       <c r="A335" s="4">
         <v>31281195846</v>
       </c>
@@ -35219,7 +35219,7 @@
       <c r="AC335" s="3"/>
       <c r="AD335" s="3"/>
     </row>
-    <row r="336" spans="1:30" ht="12.75" hidden="1">
+    <row r="336" spans="1:30" ht="12.75">
       <c r="A336" s="4">
         <v>31281195846</v>
       </c>
@@ -35299,7 +35299,7 @@
       <c r="AC336" s="3"/>
       <c r="AD336" s="3"/>
     </row>
-    <row r="337" spans="1:30" ht="12.75" hidden="1">
+    <row r="337" spans="1:30" ht="12.75">
       <c r="A337" s="4">
         <v>41281079956</v>
       </c>
@@ -35379,7 +35379,7 @@
       <c r="AC337" s="3"/>
       <c r="AD337" s="3"/>
     </row>
-    <row r="338" spans="1:30" ht="12.75" hidden="1">
+    <row r="338" spans="1:30" ht="12.75">
       <c r="A338" s="4">
         <v>31281195846</v>
       </c>
@@ -35459,7 +35459,7 @@
       <c r="AC338" s="3"/>
       <c r="AD338" s="3"/>
     </row>
-    <row r="339" spans="1:30" ht="12.75" hidden="1">
+    <row r="339" spans="1:30" ht="12.75">
       <c r="A339" s="4">
         <v>31281195846</v>
       </c>
@@ -35539,7 +35539,7 @@
       <c r="AC339" s="3"/>
       <c r="AD339" s="3"/>
     </row>
-    <row r="340" spans="1:30" ht="12.75" hidden="1">
+    <row r="340" spans="1:30" ht="12.75">
       <c r="A340" s="4">
         <v>31281195846</v>
       </c>
@@ -35619,7 +35619,7 @@
       <c r="AC340" s="3"/>
       <c r="AD340" s="3"/>
     </row>
-    <row r="341" spans="1:30" ht="12.75" hidden="1">
+    <row r="341" spans="1:30" ht="12.75">
       <c r="A341" s="4">
         <v>31281195846</v>
       </c>
@@ -35699,7 +35699,7 @@
       <c r="AC341" s="3"/>
       <c r="AD341" s="3"/>
     </row>
-    <row r="342" spans="1:30" ht="12.75" hidden="1">
+    <row r="342" spans="1:30" ht="12.75">
       <c r="A342" s="4">
         <v>31281195846</v>
       </c>
@@ -35779,7 +35779,7 @@
       <c r="AC342" s="3"/>
       <c r="AD342" s="3"/>
     </row>
-    <row r="343" spans="1:30" ht="12.75" hidden="1">
+    <row r="343" spans="1:30" ht="12.75">
       <c r="A343" s="4">
         <v>31281195846</v>
       </c>
@@ -35859,7 +35859,7 @@
       <c r="AC343" s="3"/>
       <c r="AD343" s="3"/>
     </row>
-    <row r="344" spans="1:30" ht="12.75" hidden="1">
+    <row r="344" spans="1:30" ht="12.75">
       <c r="A344" s="4">
         <v>31281195846</v>
       </c>
@@ -35939,7 +35939,7 @@
       <c r="AC344" s="3"/>
       <c r="AD344" s="3"/>
     </row>
-    <row r="345" spans="1:30" ht="12.75" hidden="1">
+    <row r="345" spans="1:30" ht="12.75">
       <c r="A345" s="4">
         <v>31281195846</v>
       </c>
@@ -36019,7 +36019,7 @@
       <c r="AC345" s="3"/>
       <c r="AD345" s="3"/>
     </row>
-    <row r="346" spans="1:30" ht="12.75" hidden="1">
+    <row r="346" spans="1:30" ht="12.75">
       <c r="A346" s="4">
         <v>20181651916</v>
       </c>
@@ -36099,7 +36099,7 @@
       <c r="AC346" s="3"/>
       <c r="AD346" s="3"/>
     </row>
-    <row r="347" spans="1:30" ht="12.75" hidden="1">
+    <row r="347" spans="1:30" ht="12.75">
       <c r="A347" s="4">
         <v>31281195846</v>
       </c>
@@ -36179,7 +36179,7 @@
       <c r="AC347" s="3"/>
       <c r="AD347" s="3"/>
     </row>
-    <row r="348" spans="1:30" ht="12.75" hidden="1">
+    <row r="348" spans="1:30" ht="12.75">
       <c r="A348" s="4">
         <v>31081061806</v>
       </c>
@@ -36259,7 +36259,7 @@
       <c r="AC348" s="3"/>
       <c r="AD348" s="3"/>
     </row>
-    <row r="349" spans="1:30" ht="12.75" hidden="1">
+    <row r="349" spans="1:30" ht="12.75">
       <c r="A349" s="4">
         <v>91204354277</v>
       </c>
@@ -36339,7 +36339,7 @@
       <c r="AC349" s="3"/>
       <c r="AD349" s="3"/>
     </row>
-    <row r="350" spans="1:30" ht="12.75" hidden="1">
+    <row r="350" spans="1:30" ht="12.75">
       <c r="A350" s="4">
         <v>12881584876</v>
       </c>
@@ -36419,7 +36419,7 @@
       <c r="AC350" s="3"/>
       <c r="AD350" s="3"/>
     </row>
-    <row r="351" spans="1:30" ht="12.75" hidden="1">
+    <row r="351" spans="1:30" ht="12.75">
       <c r="A351" s="4">
         <v>51581336046</v>
       </c>
@@ -36493,7 +36493,7 @@
       <c r="AC351" s="3"/>
       <c r="AD351" s="3"/>
     </row>
-    <row r="352" spans="1:30" ht="12.75" hidden="1">
+    <row r="352" spans="1:30" ht="12.75">
       <c r="A352" s="4">
         <v>31281195846</v>
       </c>
@@ -36569,7 +36569,7 @@
       <c r="AC352" s="3"/>
       <c r="AD352" s="3"/>
     </row>
-    <row r="353" spans="1:30" ht="12.75" hidden="1">
+    <row r="353" spans="1:30" ht="12.75">
       <c r="A353" s="4">
         <v>51481865976</v>
       </c>
@@ -36645,7 +36645,7 @@
       <c r="AC353" s="3"/>
       <c r="AD353" s="3"/>
     </row>
-    <row r="354" spans="1:30" ht="12.75" hidden="1">
+    <row r="354" spans="1:30" ht="12.75">
       <c r="A354" s="4">
         <v>60381372706</v>
       </c>
@@ -36721,7 +36721,7 @@
       <c r="AC354" s="3"/>
       <c r="AD354" s="3"/>
     </row>
-    <row r="355" spans="1:30" ht="12.75" hidden="1">
+    <row r="355" spans="1:30" ht="12.75">
       <c r="A355" s="4">
         <v>40281141316</v>
       </c>
@@ -36795,7 +36795,7 @@
       <c r="AC355" s="3"/>
       <c r="AD355" s="3"/>
     </row>
-    <row r="356" spans="1:30" ht="12.75" hidden="1">
+    <row r="356" spans="1:30" ht="12.75">
       <c r="A356" s="4">
         <v>10181349286</v>
       </c>
@@ -36871,7 +36871,7 @@
       <c r="AC356" s="3"/>
       <c r="AD356" s="3"/>
     </row>
-    <row r="357" spans="1:30" ht="12.75" hidden="1">
+    <row r="357" spans="1:30" ht="12.75">
       <c r="A357" s="4">
         <v>10581595196</v>
       </c>
@@ -36947,7 +36947,7 @@
       <c r="AC357" s="3"/>
       <c r="AD357" s="3"/>
     </row>
-    <row r="358" spans="1:30" ht="12.75" hidden="1">
+    <row r="358" spans="1:30" ht="12.75">
       <c r="A358" s="4">
         <v>90700104187</v>
       </c>
@@ -37023,7 +37023,7 @@
       <c r="AC358" s="3"/>
       <c r="AD358" s="3"/>
     </row>
-    <row r="359" spans="1:30" ht="12.75" hidden="1">
+    <row r="359" spans="1:30" ht="12.75">
       <c r="A359" s="4">
         <v>31381351416</v>
       </c>
@@ -37099,7 +37099,7 @@
       <c r="AC359" s="3"/>
       <c r="AD359" s="3"/>
     </row>
-    <row r="360" spans="1:30" ht="12.75" hidden="1">
+    <row r="360" spans="1:30" ht="12.75">
       <c r="A360" s="4">
         <v>10181162936</v>
       </c>
@@ -37175,7 +37175,7 @@
       <c r="AC360" s="3"/>
       <c r="AD360" s="3"/>
     </row>
-    <row r="361" spans="1:30" ht="12.75" hidden="1">
+    <row r="361" spans="1:30" ht="12.75">
       <c r="A361" s="4">
         <v>41681133686</v>
       </c>
@@ -37251,7 +37251,7 @@
       <c r="AC361" s="3"/>
       <c r="AD361" s="3"/>
     </row>
-    <row r="362" spans="1:30" ht="12.75" hidden="1">
+    <row r="362" spans="1:30" ht="12.75">
       <c r="A362" s="4">
         <v>10481181216</v>
       </c>
@@ -37327,7 +37327,7 @@
       <c r="AC362" s="3"/>
       <c r="AD362" s="3"/>
     </row>
-    <row r="363" spans="1:30" ht="12.75" hidden="1">
+    <row r="363" spans="1:30" ht="12.75">
       <c r="A363" s="4">
         <v>10281317546</v>
       </c>
@@ -37403,7 +37403,7 @@
       <c r="AC363" s="3"/>
       <c r="AD363" s="3"/>
     </row>
-    <row r="364" spans="1:30" ht="12.75" hidden="1">
+    <row r="364" spans="1:30" ht="12.75">
       <c r="A364" s="4">
         <v>12681053256</v>
       </c>
@@ -37479,7 +37479,7 @@
       <c r="AC364" s="3"/>
       <c r="AD364" s="3"/>
     </row>
-    <row r="365" spans="1:30" ht="12.75" hidden="1">
+    <row r="365" spans="1:30" ht="12.75">
       <c r="A365" s="4">
         <v>72881008306</v>
       </c>
@@ -37555,7 +37555,7 @@
       <c r="AC365" s="3"/>
       <c r="AD365" s="3"/>
     </row>
-    <row r="366" spans="1:30" ht="12.75" hidden="1">
+    <row r="366" spans="1:30" ht="12.75">
       <c r="A366" s="4">
         <v>61781091906</v>
       </c>
@@ -37631,7 +37631,7 @@
       <c r="AC366" s="3"/>
       <c r="AD366" s="3"/>
     </row>
-    <row r="367" spans="1:30" ht="12.75" hidden="1">
+    <row r="367" spans="1:30" ht="12.75">
       <c r="A367" s="4">
         <v>11481609466</v>
       </c>
@@ -37707,7 +37707,7 @@
       <c r="AC367" s="3"/>
       <c r="AD367" s="3"/>
     </row>
-    <row r="368" spans="1:30" ht="12.75" hidden="1">
+    <row r="368" spans="1:30" ht="12.75">
       <c r="A368" s="4">
         <v>61081251276</v>
       </c>
@@ -37783,7 +37783,7 @@
       <c r="AC368" s="3"/>
       <c r="AD368" s="3"/>
     </row>
-    <row r="369" spans="1:30" ht="12.75" hidden="1">
+    <row r="369" spans="1:30" ht="12.75">
       <c r="A369" s="4">
         <v>51081107946</v>
       </c>
@@ -37859,7 +37859,7 @@
       <c r="AC369" s="3"/>
       <c r="AD369" s="3"/>
     </row>
-    <row r="370" spans="1:30" ht="12.75" hidden="1">
+    <row r="370" spans="1:30" ht="12.75">
       <c r="A370" s="4">
         <v>40986014386</v>
       </c>
@@ -37935,7 +37935,7 @@
       <c r="AC370" s="3"/>
       <c r="AD370" s="3"/>
     </row>
-    <row r="371" spans="1:30" ht="12.75" hidden="1">
+    <row r="371" spans="1:30" ht="12.75">
       <c r="A371" s="4">
         <v>20181456856</v>
       </c>
@@ -38011,7 +38011,7 @@
       <c r="AC371" s="3"/>
       <c r="AD371" s="3"/>
     </row>
-    <row r="372" spans="1:30" ht="12.75" hidden="1">
+    <row r="372" spans="1:30" ht="12.75">
       <c r="A372" s="4">
         <v>90700104187</v>
       </c>
@@ -38087,7 +38087,7 @@
       <c r="AC372" s="3"/>
       <c r="AD372" s="3"/>
     </row>
-    <row r="373" spans="1:30" ht="12.75" hidden="1">
+    <row r="373" spans="1:30" ht="12.75">
       <c r="A373" s="4">
         <v>60581164186</v>
       </c>
@@ -38163,7 +38163,7 @@
       <c r="AC373" s="3"/>
       <c r="AD373" s="3"/>
     </row>
-    <row r="374" spans="1:30" ht="12.75" hidden="1">
+    <row r="374" spans="1:30" ht="12.75">
       <c r="A374" s="4">
         <v>40881099606</v>
       </c>
@@ -38237,7 +38237,7 @@
       <c r="AC374" s="3"/>
       <c r="AD374" s="3"/>
     </row>
-    <row r="375" spans="1:30" ht="12.75" hidden="1">
+    <row r="375" spans="1:30" ht="12.75">
       <c r="A375" s="4">
         <v>13186586306</v>
       </c>
@@ -38313,7 +38313,7 @@
       <c r="AC375" s="3"/>
       <c r="AD375" s="3"/>
     </row>
-    <row r="376" spans="1:30" ht="12.75" hidden="1">
+    <row r="376" spans="1:30" ht="12.75">
       <c r="A376" s="4">
         <v>12281282916</v>
       </c>
@@ -38389,7 +38389,7 @@
       <c r="AC376" s="3"/>
       <c r="AD376" s="3"/>
     </row>
-    <row r="377" spans="1:30" ht="12.75" hidden="1">
+    <row r="377" spans="1:30" ht="12.75">
       <c r="A377" s="4">
         <v>10581676446</v>
       </c>
@@ -38465,7 +38465,7 @@
       <c r="AC377" s="3"/>
       <c r="AD377" s="3"/>
     </row>
-    <row r="378" spans="1:30" ht="12.75" hidden="1">
+    <row r="378" spans="1:30" ht="12.75">
       <c r="A378" s="4">
         <v>10281317546</v>
       </c>
@@ -38541,7 +38541,7 @@
       <c r="AC378" s="3"/>
       <c r="AD378" s="3"/>
     </row>
-    <row r="379" spans="1:30" ht="12.75" hidden="1">
+    <row r="379" spans="1:30" ht="12.75">
       <c r="A379" s="4">
         <v>61786174676</v>
       </c>
@@ -38615,7 +38615,7 @@
       <c r="AC379" s="3"/>
       <c r="AD379" s="3"/>
     </row>
-    <row r="380" spans="1:30" ht="12.75" hidden="1">
+    <row r="380" spans="1:30" ht="12.75">
       <c r="A380" s="4">
         <v>22981197736</v>
       </c>
@@ -38689,7 +38689,7 @@
       <c r="AC380" s="3"/>
       <c r="AD380" s="3"/>
     </row>
-    <row r="381" spans="1:30" ht="12.75" hidden="1">
+    <row r="381" spans="1:30" ht="12.75">
       <c r="A381" s="4">
         <v>12881132726</v>
       </c>
@@ -38763,7 +38763,7 @@
       <c r="AC381" s="3"/>
       <c r="AD381" s="3"/>
     </row>
-    <row r="382" spans="1:30" ht="12.75" hidden="1">
+    <row r="382" spans="1:30" ht="12.75">
       <c r="A382" s="4">
         <v>90700104187</v>
       </c>
@@ -38837,7 +38837,7 @@
       <c r="AC382" s="3"/>
       <c r="AD382" s="3"/>
     </row>
-    <row r="383" spans="1:30" ht="12.75" hidden="1">
+    <row r="383" spans="1:30" ht="12.75">
       <c r="A383" s="4">
         <v>13881206876</v>
       </c>
@@ -38911,7 +38911,7 @@
       <c r="AC383" s="3"/>
       <c r="AD383" s="3"/>
     </row>
-    <row r="384" spans="1:30" ht="12.75" hidden="1">
+    <row r="384" spans="1:30" ht="12.75">
       <c r="A384" s="4">
         <v>13881774586</v>
       </c>
@@ -38985,7 +38985,7 @@
       <c r="AC384" s="3"/>
       <c r="AD384" s="3"/>
     </row>
-    <row r="385" spans="1:30" ht="12.75" hidden="1">
+    <row r="385" spans="1:30" ht="12.75">
       <c r="A385" s="4">
         <v>10181162936</v>
       </c>
@@ -39059,7 +39059,7 @@
       <c r="AC385" s="3"/>
       <c r="AD385" s="3"/>
     </row>
-    <row r="386" spans="1:30" ht="12.75" hidden="1">
+    <row r="386" spans="1:30" ht="12.75">
       <c r="A386" s="4">
         <v>10481181216</v>
       </c>
@@ -39133,7 +39133,7 @@
       <c r="AC386" s="3"/>
       <c r="AD386" s="3"/>
     </row>
-    <row r="387" spans="1:30" ht="12.75" hidden="1">
+    <row r="387" spans="1:30" ht="12.75">
       <c r="A387" s="4">
         <v>90700104187</v>
       </c>
@@ -39207,7 +39207,7 @@
       <c r="AC387" s="3"/>
       <c r="AD387" s="3"/>
     </row>
-    <row r="388" spans="1:30" ht="12.75" hidden="1">
+    <row r="388" spans="1:30" ht="12.75">
       <c r="A388" s="4">
         <v>11481163776</v>
       </c>
@@ -39281,7 +39281,7 @@
       <c r="AC388" s="3"/>
       <c r="AD388" s="3"/>
     </row>
-    <row r="389" spans="1:30" ht="12.75" hidden="1">
+    <row r="389" spans="1:30" ht="12.75">
       <c r="A389" s="4">
         <v>13486935436</v>
       </c>
@@ -39355,7 +39355,7 @@
       <c r="AC389" s="3"/>
       <c r="AD389" s="3"/>
     </row>
-    <row r="390" spans="1:30" ht="12.75" hidden="1">
+    <row r="390" spans="1:30" ht="12.75">
       <c r="A390" s="4">
         <v>31286752236</v>
       </c>
@@ -39429,7 +39429,7 @@
       <c r="AC390" s="3"/>
       <c r="AD390" s="3"/>
     </row>
-    <row r="391" spans="1:30" ht="12.75" hidden="1">
+    <row r="391" spans="1:30" ht="12.75">
       <c r="A391" s="4">
         <v>90700104187</v>
       </c>
@@ -39503,7 +39503,7 @@
       <c r="AC391" s="3"/>
       <c r="AD391" s="3"/>
     </row>
-    <row r="392" spans="1:30" ht="12.75" hidden="1">
+    <row r="392" spans="1:30" ht="12.75">
       <c r="A392" s="4">
         <v>13881085346</v>
       </c>
@@ -39575,7 +39575,7 @@
       <c r="AC392" s="3"/>
       <c r="AD392" s="3"/>
     </row>
-    <row r="393" spans="1:30" ht="12.75" hidden="1">
+    <row r="393" spans="1:30" ht="12.75">
       <c r="A393" s="4">
         <v>61081533566</v>
       </c>
@@ -39649,7 +39649,7 @@
       <c r="AC393" s="3"/>
       <c r="AD393" s="3"/>
     </row>
-    <row r="394" spans="1:30" ht="12.75" hidden="1">
+    <row r="394" spans="1:30" ht="12.75">
       <c r="A394" s="4">
         <v>12086216766</v>
       </c>
@@ -39723,7 +39723,7 @@
       <c r="AC394" s="3"/>
       <c r="AD394" s="3"/>
     </row>
-    <row r="395" spans="1:30" ht="12.75" hidden="1">
+    <row r="395" spans="1:30" ht="12.75">
       <c r="A395" s="4">
         <v>20981104776</v>
       </c>
@@ -39797,7 +39797,7 @@
       <c r="AC395" s="3"/>
       <c r="AD395" s="3"/>
     </row>
-    <row r="396" spans="1:30" ht="12.75" hidden="1">
+    <row r="396" spans="1:30" ht="12.75">
       <c r="A396" s="4">
         <v>10181162936</v>
       </c>
@@ -39871,7 +39871,7 @@
       <c r="AC396" s="3"/>
       <c r="AD396" s="3"/>
     </row>
-    <row r="397" spans="1:30" ht="12.75" hidden="1">
+    <row r="397" spans="1:30" ht="12.75">
       <c r="A397" s="4">
         <v>20281459756</v>
       </c>
@@ -39943,7 +39943,7 @@
       <c r="AC397" s="3"/>
       <c r="AD397" s="3"/>
     </row>
-    <row r="398" spans="1:30" ht="12.75" hidden="1">
+    <row r="398" spans="1:30" ht="12.75">
       <c r="A398" s="4">
         <v>10281317546</v>
       </c>
@@ -40017,7 +40017,7 @@
       <c r="AC398" s="3"/>
       <c r="AD398" s="3"/>
     </row>
-    <row r="399" spans="1:30" ht="12.75" hidden="1">
+    <row r="399" spans="1:30" ht="12.75">
       <c r="A399" s="4">
         <v>88381002866</v>
       </c>
@@ -40091,7 +40091,7 @@
       <c r="AC399" s="3"/>
       <c r="AD399" s="3"/>
     </row>
-    <row r="400" spans="1:30" ht="12.75" hidden="1">
+    <row r="400" spans="1:30" ht="12.75">
       <c r="A400" s="4">
         <v>91204354277</v>
       </c>
@@ -40165,7 +40165,7 @@
       <c r="AC400" s="3"/>
       <c r="AD400" s="3"/>
     </row>
-    <row r="401" spans="1:30" ht="12.75" hidden="1">
+    <row r="401" spans="1:30" ht="12.75">
       <c r="A401" s="4">
         <v>30881043796</v>
       </c>
@@ -40243,7 +40243,7 @@
       <c r="AC401" s="3"/>
       <c r="AD401" s="3"/>
     </row>
-    <row r="402" spans="1:30" ht="12.75" hidden="1">
+    <row r="402" spans="1:30" ht="12.75">
       <c r="A402" s="4">
         <v>60781721916</v>
       </c>
@@ -40321,7 +40321,7 @@
       <c r="AC402" s="3"/>
       <c r="AD402" s="3"/>
     </row>
-    <row r="403" spans="1:30" ht="12.75" hidden="1">
+    <row r="403" spans="1:30" ht="12.75">
       <c r="A403" s="4">
         <v>21481699656</v>
       </c>
@@ -40399,7 +40399,7 @@
       <c r="AC403" s="3"/>
       <c r="AD403" s="3"/>
     </row>
-    <row r="404" spans="1:30" ht="12.75" hidden="1">
+    <row r="404" spans="1:30" ht="12.75">
       <c r="A404" s="4">
         <v>40881982696</v>
       </c>
@@ -40477,7 +40477,7 @@
       <c r="AC404" s="3"/>
       <c r="AD404" s="3"/>
     </row>
-    <row r="405" spans="1:30" ht="12.75" hidden="1">
+    <row r="405" spans="1:30" ht="12.75">
       <c r="A405" s="4">
         <v>12886283006</v>
       </c>
@@ -40555,7 +40555,7 @@
       <c r="AC405" s="3"/>
       <c r="AD405" s="3"/>
     </row>
-    <row r="406" spans="1:30" ht="12.75" hidden="1">
+    <row r="406" spans="1:30" ht="12.75">
       <c r="A406" s="4">
         <v>11481163776</v>
       </c>
@@ -40633,7 +40633,7 @@
       <c r="AC406" s="3"/>
       <c r="AD406" s="3"/>
     </row>
-    <row r="407" spans="1:30" ht="12.75" hidden="1">
+    <row r="407" spans="1:30" ht="12.75">
       <c r="A407" s="4">
         <v>10581595196</v>
       </c>
@@ -40711,7 +40711,7 @@
       <c r="AC407" s="3"/>
       <c r="AD407" s="3"/>
     </row>
-    <row r="408" spans="1:30" ht="12.75" hidden="1">
+    <row r="408" spans="1:30" ht="12.75">
       <c r="A408" s="4">
         <v>11081146116</v>
       </c>
@@ -40789,7 +40789,7 @@
       <c r="AC408" s="3"/>
       <c r="AD408" s="3"/>
     </row>
-    <row r="409" spans="1:30" ht="12.75" hidden="1">
+    <row r="409" spans="1:30" ht="12.75">
       <c r="A409" s="4">
         <v>88788009296</v>
       </c>
@@ -40867,7 +40867,7 @@
       <c r="AC409" s="3"/>
       <c r="AD409" s="3"/>
     </row>
-    <row r="410" spans="1:30" ht="12.75" hidden="1">
+    <row r="410" spans="1:30" ht="12.75">
       <c r="A410" s="4">
         <v>10481181216</v>
       </c>
@@ -40945,7 +40945,7 @@
       <c r="AC410" s="3"/>
       <c r="AD410" s="3"/>
     </row>
-    <row r="411" spans="1:30" ht="12.75" hidden="1">
+    <row r="411" spans="1:30" ht="12.75">
       <c r="A411" s="4">
         <v>10181667556</v>
       </c>
@@ -41021,7 +41021,7 @@
       <c r="AC411" s="3"/>
       <c r="AD411" s="3"/>
     </row>
-    <row r="412" spans="1:30" ht="12.75" hidden="1">
+    <row r="412" spans="1:30" ht="12.75">
       <c r="A412" s="4">
         <v>10181667556</v>
       </c>
@@ -41095,7 +41095,7 @@
       <c r="AC412" s="3"/>
       <c r="AD412" s="3"/>
     </row>
-    <row r="413" spans="1:30" ht="12.75" hidden="1">
+    <row r="413" spans="1:30" ht="12.75">
       <c r="A413" s="4">
         <v>12081019576</v>
       </c>
@@ -41173,7 +41173,7 @@
       <c r="AC413" s="3"/>
       <c r="AD413" s="3"/>
     </row>
-    <row r="414" spans="1:30" ht="12.75" hidden="1">
+    <row r="414" spans="1:30" ht="12.75">
       <c r="A414" s="4">
         <v>31381028066</v>
       </c>
@@ -41251,7 +41251,7 @@
       <c r="AC414" s="3"/>
       <c r="AD414" s="3"/>
     </row>
-    <row r="415" spans="1:30" ht="12.75" hidden="1">
+    <row r="415" spans="1:30" ht="12.75">
       <c r="A415" s="4">
         <v>10281345616</v>
       </c>
@@ -41329,7 +41329,7 @@
       <c r="AC415" s="3"/>
       <c r="AD415" s="3"/>
     </row>
-    <row r="416" spans="1:30" ht="12.75" hidden="1">
+    <row r="416" spans="1:30" ht="12.75">
       <c r="A416" s="4">
         <v>40881452346</v>
       </c>
@@ -41407,7 +41407,7 @@
       <c r="AC416" s="3"/>
       <c r="AD416" s="3"/>
     </row>
-    <row r="417" spans="1:30" ht="12.75" hidden="1">
+    <row r="417" spans="1:30" ht="12.75">
       <c r="A417" s="4">
         <v>31481079546</v>
       </c>
@@ -41485,7 +41485,7 @@
       <c r="AC417" s="3"/>
       <c r="AD417" s="3"/>
     </row>
-    <row r="418" spans="1:30" ht="12.75" hidden="1">
+    <row r="418" spans="1:30" ht="12.75">
       <c r="A418" s="4">
         <v>10181667556</v>
       </c>
@@ -41561,7 +41561,7 @@
       <c r="AC418" s="3"/>
       <c r="AD418" s="3"/>
     </row>
-    <row r="419" spans="1:30" ht="12.75" hidden="1">
+    <row r="419" spans="1:30" ht="12.75">
       <c r="A419" s="4">
         <v>60681711466</v>
       </c>
@@ -41639,7 +41639,7 @@
       <c r="AC419" s="3"/>
       <c r="AD419" s="3"/>
     </row>
-    <row r="420" spans="1:30" ht="12.75" hidden="1">
+    <row r="420" spans="1:30" ht="12.75">
       <c r="A420" s="4">
         <v>10181162936</v>
       </c>
@@ -41717,7 +41717,7 @@
       <c r="AC420" s="3"/>
       <c r="AD420" s="3"/>
     </row>
-    <row r="421" spans="1:30" ht="12.75" hidden="1">
+    <row r="421" spans="1:30" ht="12.75">
       <c r="A421" s="4">
         <v>10181162936</v>
       </c>
@@ -41795,7 +41795,7 @@
       <c r="AC421" s="3"/>
       <c r="AD421" s="3"/>
     </row>
-    <row r="422" spans="1:30" ht="12.75" hidden="1">
+    <row r="422" spans="1:30" ht="12.75">
       <c r="A422" s="4">
         <v>10181162936</v>
       </c>
@@ -41873,7 +41873,7 @@
       <c r="AC422" s="3"/>
       <c r="AD422" s="3"/>
     </row>
-    <row r="423" spans="1:30" ht="12.75" hidden="1">
+    <row r="423" spans="1:30" ht="12.75">
       <c r="A423" s="4">
         <v>11481588536</v>
       </c>
@@ -41949,7 +41949,7 @@
       <c r="AC423" s="3"/>
       <c r="AD423" s="3"/>
     </row>
-    <row r="424" spans="1:30" ht="12.75" hidden="1">
+    <row r="424" spans="1:30" ht="12.75">
       <c r="A424" s="4">
         <v>11481588536</v>
       </c>
@@ -42025,7 +42025,7 @@
       <c r="AC424" s="3"/>
       <c r="AD424" s="3"/>
     </row>
-    <row r="425" spans="1:30" ht="12.75" hidden="1">
+    <row r="425" spans="1:30" ht="12.75">
       <c r="A425" s="4">
         <v>11481588536</v>
       </c>
@@ -42101,7 +42101,7 @@
       <c r="AC425" s="3"/>
       <c r="AD425" s="3"/>
     </row>
-    <row r="426" spans="1:30" ht="12.75" hidden="1">
+    <row r="426" spans="1:30" ht="12.75">
       <c r="A426" s="4">
         <v>91405877877</v>
       </c>
@@ -42179,7 +42179,7 @@
       <c r="AC426" s="3"/>
       <c r="AD426" s="3"/>
     </row>
-    <row r="427" spans="1:30" ht="12.75" hidden="1">
+    <row r="427" spans="1:30" ht="12.75">
       <c r="A427" s="4">
         <v>11481588536</v>
       </c>
@@ -42255,7 +42255,7 @@
       <c r="AC427" s="3"/>
       <c r="AD427" s="3"/>
     </row>
-    <row r="428" spans="1:30" ht="12.75" hidden="1">
+    <row r="428" spans="1:30" ht="12.75">
       <c r="A428" s="4">
         <v>11481588536</v>
       </c>
@@ -42331,7 +42331,7 @@
       <c r="AC428" s="3"/>
       <c r="AD428" s="3"/>
     </row>
-    <row r="429" spans="1:30" ht="12.75" hidden="1">
+    <row r="429" spans="1:30" ht="12.75">
       <c r="A429" s="4">
         <v>11481588536</v>
       </c>
@@ -42407,7 +42407,7 @@
       <c r="AC429" s="3"/>
       <c r="AD429" s="3"/>
     </row>
-    <row r="430" spans="1:30" ht="12.75" hidden="1">
+    <row r="430" spans="1:30" ht="12.75">
       <c r="A430" s="4">
         <v>12686390776</v>
       </c>
@@ -42485,7 +42485,7 @@
       <c r="AC430" s="3"/>
       <c r="AD430" s="3"/>
     </row>
-    <row r="431" spans="1:30" ht="12.75" hidden="1">
+    <row r="431" spans="1:30" ht="12.75">
       <c r="A431" s="4">
         <v>85388001736</v>
       </c>
@@ -42563,7 +42563,7 @@
       <c r="AC431" s="3"/>
       <c r="AD431" s="3"/>
     </row>
-    <row r="432" spans="1:30" ht="12.75" hidden="1">
+    <row r="432" spans="1:30" ht="12.75">
       <c r="A432" s="4">
         <v>31581011046</v>
       </c>
@@ -42641,7 +42641,7 @@
       <c r="AC432" s="3"/>
       <c r="AD432" s="3"/>
     </row>
-    <row r="433" spans="1:30" ht="12.75" hidden="1">
+    <row r="433" spans="1:30" ht="12.75">
       <c r="A433" s="4">
         <v>21281628936</v>
       </c>
@@ -42719,7 +42719,7 @@
       <c r="AC433" s="3"/>
       <c r="AD433" s="3"/>
     </row>
-    <row r="434" spans="1:30" ht="12.75" hidden="1">
+    <row r="434" spans="1:30" ht="12.75">
       <c r="A434" s="4">
         <v>11681415906</v>
       </c>
@@ -42795,7 +42795,7 @@
       <c r="AC434" s="3"/>
       <c r="AD434" s="3"/>
     </row>
-    <row r="435" spans="1:30" ht="12.75" hidden="1">
+    <row r="435" spans="1:30" ht="12.75">
       <c r="A435" s="4">
         <v>60981135436</v>
       </c>
@@ -42873,7 +42873,7 @@
       <c r="AC435" s="3"/>
       <c r="AD435" s="3"/>
     </row>
-    <row r="436" spans="1:30" ht="12.75" hidden="1">
+    <row r="436" spans="1:30" ht="12.75">
       <c r="A436" s="4">
         <v>11681350076</v>
       </c>
@@ -42947,7 +42947,7 @@
       <c r="AC436" s="3"/>
       <c r="AD436" s="3"/>
     </row>
-    <row r="437" spans="1:30" ht="12.75" hidden="1">
+    <row r="437" spans="1:30" ht="12.75">
       <c r="A437" s="4">
         <v>90700104187</v>
       </c>
@@ -43025,7 +43025,7 @@
       <c r="AC437" s="3"/>
       <c r="AD437" s="3"/>
     </row>
-    <row r="438" spans="1:30" ht="12.75" hidden="1">
+    <row r="438" spans="1:30" ht="12.75">
       <c r="A438" s="4">
         <v>11381446766</v>
       </c>
@@ -43103,7 +43103,7 @@
       <c r="AC438" s="3"/>
       <c r="AD438" s="3"/>
     </row>
-    <row r="439" spans="1:30" ht="12.75" hidden="1">
+    <row r="439" spans="1:30" ht="12.75">
       <c r="A439" s="4">
         <v>22481113976</v>
       </c>
@@ -43181,7 +43181,7 @@
       <c r="AC439" s="3"/>
       <c r="AD439" s="3"/>
     </row>
-    <row r="440" spans="1:30" ht="12.75" hidden="1">
+    <row r="440" spans="1:30" ht="12.75">
       <c r="A440" s="4">
         <v>91813373377</v>
       </c>
@@ -43259,7 +43259,7 @@
       <c r="AC440" s="3"/>
       <c r="AD440" s="3"/>
     </row>
-    <row r="441" spans="1:30" ht="12.75" hidden="1">
+    <row r="441" spans="1:30" ht="12.75">
       <c r="A441" s="4">
         <v>10181349286</v>
       </c>
@@ -43335,7 +43335,7 @@
       <c r="AC441" s="3"/>
       <c r="AD441" s="3"/>
     </row>
-    <row r="442" spans="1:30" ht="12.75" hidden="1">
+    <row r="442" spans="1:30" ht="12.75">
       <c r="A442" s="4">
         <v>10181162936</v>
       </c>
@@ -43413,7 +43413,7 @@
       <c r="AC442" s="3"/>
       <c r="AD442" s="3"/>
     </row>
-    <row r="443" spans="1:30" ht="12.75" hidden="1">
+    <row r="443" spans="1:30" ht="12.75">
       <c r="A443" s="4">
         <v>11081050346</v>
       </c>
@@ -43489,7 +43489,7 @@
       <c r="AC443" s="3"/>
       <c r="AD443" s="3"/>
     </row>
-    <row r="444" spans="1:30" ht="12.75" hidden="1">
+    <row r="444" spans="1:30" ht="12.75">
       <c r="A444" s="4">
         <v>12881584876</v>
       </c>
@@ -43567,7 +43567,7 @@
       <c r="AC444" s="3"/>
       <c r="AD444" s="3"/>
     </row>
-    <row r="445" spans="1:30" ht="12.75" hidden="1">
+    <row r="445" spans="1:30" ht="12.75">
       <c r="A445" s="4">
         <v>21487358846</v>
       </c>
@@ -43643,7 +43643,7 @@
       <c r="AC445" s="3"/>
       <c r="AD445" s="3"/>
     </row>
-    <row r="446" spans="1:30" ht="12.75" hidden="1">
+    <row r="446" spans="1:30" ht="12.75">
       <c r="A446" s="4">
         <v>30181311576</v>
       </c>
@@ -43721,7 +43721,7 @@
       <c r="AC446" s="3"/>
       <c r="AD446" s="3"/>
     </row>
-    <row r="447" spans="1:30" ht="12.75" hidden="1">
+    <row r="447" spans="1:30" ht="12.75">
       <c r="A447" s="4">
         <v>50181000506</v>
       </c>
@@ -43799,7 +43799,7 @@
       <c r="AC447" s="3"/>
       <c r="AD447" s="3"/>
     </row>
-    <row r="448" spans="1:30" ht="12.75" hidden="1">
+    <row r="448" spans="1:30" ht="12.75">
       <c r="A448" s="4">
         <v>10281317546</v>
       </c>
@@ -43877,7 +43877,7 @@
       <c r="AC448" s="3"/>
       <c r="AD448" s="3"/>
     </row>
-    <row r="449" spans="1:30" ht="12.75" hidden="1">
+    <row r="449" spans="1:30" ht="12.75">
       <c r="A449" s="4">
         <v>14181277076</v>
       </c>
@@ -43953,7 +43953,7 @@
       <c r="AC449" s="3"/>
       <c r="AD449" s="3"/>
     </row>
-    <row r="450" spans="1:30" ht="12.75" hidden="1">
+    <row r="450" spans="1:30" ht="12.75">
       <c r="A450" s="4">
         <v>41881058076</v>
       </c>
@@ -44031,7 +44031,7 @@
       <c r="AC450" s="3"/>
       <c r="AD450" s="3"/>
     </row>
-    <row r="451" spans="1:30" ht="12.75" hidden="1">
+    <row r="451" spans="1:30" ht="12.75">
       <c r="A451" s="4">
         <v>90700104187</v>
       </c>
@@ -44109,7 +44109,7 @@
       <c r="AC451" s="3"/>
       <c r="AD451" s="3"/>
     </row>
-    <row r="452" spans="1:30" ht="12.75" hidden="1">
+    <row r="452" spans="1:30" ht="12.75">
       <c r="A452" s="4">
         <v>60181184906</v>
       </c>
@@ -44187,7 +44187,7 @@
       <c r="AC452" s="3"/>
       <c r="AD452" s="3"/>
     </row>
-    <row r="453" spans="1:30" ht="12.75" hidden="1">
+    <row r="453" spans="1:30" ht="12.75">
       <c r="A453" s="4">
         <v>11481163776</v>
       </c>
@@ -44265,7 +44265,7 @@
       <c r="AC453" s="3"/>
       <c r="AD453" s="3"/>
     </row>
-    <row r="454" spans="1:30" ht="12.75" hidden="1">
+    <row r="454" spans="1:30" ht="12.75">
       <c r="A454" s="4">
         <v>50281554656</v>
       </c>
@@ -44343,7 +44343,7 @@
       <c r="AC454" s="3"/>
       <c r="AD454" s="3"/>
     </row>
-    <row r="455" spans="1:30" ht="12.75" hidden="1">
+    <row r="455" spans="1:30" ht="12.75">
       <c r="A455" s="4">
         <v>11681350076</v>
       </c>
@@ -44417,7 +44417,7 @@
       <c r="AC455" s="3"/>
       <c r="AD455" s="3"/>
     </row>
-    <row r="456" spans="1:30" ht="12.75" hidden="1">
+    <row r="456" spans="1:30" ht="12.75">
       <c r="A456" s="4">
         <v>41086447236</v>
       </c>
@@ -44495,7 +44495,7 @@
       <c r="AC456" s="3"/>
       <c r="AD456" s="3"/>
     </row>
-    <row r="457" spans="1:30" ht="12.75" hidden="1">
+    <row r="457" spans="1:30" ht="12.75">
       <c r="A457" s="4">
         <v>41086447236</v>
       </c>
@@ -44573,7 +44573,7 @@
       <c r="AC457" s="3"/>
       <c r="AD457" s="3"/>
     </row>
-    <row r="458" spans="1:30" ht="12.75" hidden="1">
+    <row r="458" spans="1:30" ht="12.75">
       <c r="A458" s="4">
         <v>61781084206</v>
       </c>
@@ -44651,7 +44651,7 @@
       <c r="AC458" s="3"/>
       <c r="AD458" s="3"/>
     </row>
-    <row r="459" spans="1:30" ht="12.75" hidden="1">
+    <row r="459" spans="1:30" ht="12.75">
       <c r="A459" s="4">
         <v>11481163776</v>
       </c>
@@ -44729,7 +44729,7 @@
       <c r="AC459" s="3"/>
       <c r="AD459" s="3"/>
     </row>
-    <row r="460" spans="1:30" ht="12.75" hidden="1">
+    <row r="460" spans="1:30" ht="12.75">
       <c r="A460" s="4">
         <v>11481163776</v>
       </c>
@@ -44807,7 +44807,7 @@
       <c r="AC460" s="3"/>
       <c r="AD460" s="3"/>
     </row>
-    <row r="461" spans="1:30" ht="12.75" hidden="1">
+    <row r="461" spans="1:30" ht="12.75">
       <c r="A461" s="4">
         <v>51581336046</v>
       </c>
@@ -44883,7 +44883,7 @@
       <c r="AC461" s="3"/>
       <c r="AD461" s="3"/>
     </row>
-    <row r="462" spans="1:30" ht="12.75" hidden="1">
+    <row r="462" spans="1:30" ht="12.75">
       <c r="A462" s="4">
         <v>10481181216</v>
       </c>
@@ -44959,7 +44959,7 @@
       <c r="AC462" s="3"/>
       <c r="AD462" s="3"/>
     </row>
-    <row r="463" spans="1:30" ht="12.75" hidden="1">
+    <row r="463" spans="1:30" ht="12.75">
       <c r="A463" s="4">
         <v>17386002056</v>
       </c>
@@ -45033,7 +45033,7 @@
       <c r="AC463" s="3"/>
       <c r="AD463" s="3"/>
     </row>
-    <row r="464" spans="1:30" ht="12.75" hidden="1">
+    <row r="464" spans="1:30" ht="12.75">
       <c r="A464" s="4">
         <v>50886012826</v>
       </c>
@@ -45107,7 +45107,7 @@
       <c r="AC464" s="3"/>
       <c r="AD464" s="3"/>
     </row>
-    <row r="465" spans="1:30" ht="12.75" hidden="1">
+    <row r="465" spans="1:30" ht="12.75">
       <c r="A465" s="4">
         <v>11486387216</v>
       </c>
@@ -45181,7 +45181,7 @@
       <c r="AC465" s="3"/>
       <c r="AD465" s="3"/>
     </row>
-    <row r="466" spans="1:30" ht="12.75" hidden="1">
+    <row r="466" spans="1:30" ht="12.75">
       <c r="A466" s="4">
         <v>23181049916</v>
       </c>
@@ -45255,7 +45255,7 @@
       <c r="AC466" s="3"/>
       <c r="AD466" s="3"/>
     </row>
-    <row r="467" spans="1:30" ht="12.75" hidden="1">
+    <row r="467" spans="1:30" ht="12.75">
       <c r="A467" s="4">
         <v>59087016006</v>
       </c>
@@ -45329,7 +45329,7 @@
       <c r="AC467" s="3"/>
       <c r="AD467" s="3"/>
     </row>
-    <row r="468" spans="1:30" ht="12.75" hidden="1">
+    <row r="468" spans="1:30" ht="12.75">
       <c r="A468" s="4">
         <v>20281459756</v>
       </c>
@@ -45403,7 +45403,7 @@
       <c r="AC468" s="3"/>
       <c r="AD468" s="3"/>
     </row>
-    <row r="469" spans="1:30" ht="12.75" hidden="1">
+    <row r="469" spans="1:30" ht="12.75">
       <c r="A469" s="4">
         <v>11681350076</v>
       </c>
@@ -45473,7 +45473,7 @@
       <c r="AC469" s="3"/>
       <c r="AD469" s="3"/>
     </row>
-    <row r="470" spans="1:30" ht="12.75" hidden="1">
+    <row r="470" spans="1:30" ht="12.75">
       <c r="A470" s="4">
         <v>41681133686</v>
       </c>
@@ -45549,7 +45549,7 @@
       <c r="AC470" s="3"/>
       <c r="AD470" s="3"/>
     </row>
-    <row r="471" spans="1:30" ht="12.75" hidden="1">
+    <row r="471" spans="1:30" ht="12.75">
       <c r="A471" s="4">
         <v>22081193306</v>
       </c>
@@ -45625,7 +45625,7 @@
       <c r="AC471" s="3"/>
       <c r="AD471" s="3"/>
     </row>
-    <row r="472" spans="1:30" ht="12.75" hidden="1">
+    <row r="472" spans="1:30" ht="12.75">
       <c r="A472" s="4">
         <v>40981084366</v>
       </c>
@@ -45699,7 +45699,7 @@
       <c r="AC472" s="3"/>
       <c r="AD472" s="3"/>
     </row>
-    <row r="473" spans="1:30" ht="12.75" hidden="1">
+    <row r="473" spans="1:30" ht="12.75">
       <c r="A473" s="4">
         <v>22481113976</v>
       </c>
@@ -45773,7 +45773,7 @@
       <c r="AC473" s="3"/>
       <c r="AD473" s="3"/>
     </row>
-    <row r="474" spans="1:30" ht="12.75" hidden="1">
+    <row r="474" spans="1:30" ht="12.75">
       <c r="A474" s="4">
         <v>22081109506</v>
       </c>
@@ -45849,7 +45849,7 @@
       <c r="AC474" s="3"/>
       <c r="AD474" s="3"/>
     </row>
-    <row r="475" spans="1:30" ht="12.75" hidden="1">
+    <row r="475" spans="1:30" ht="12.75">
       <c r="A475" s="4">
         <v>10581783076</v>
       </c>
@@ -45925,7 +45925,7 @@
       <c r="AC475" s="3"/>
       <c r="AD475" s="3"/>
     </row>
-    <row r="476" spans="1:30" ht="12.75" hidden="1">
+    <row r="476" spans="1:30" ht="12.75">
       <c r="A476" s="4">
         <v>12881632626</v>
       </c>
@@ -46001,7 +46001,7 @@
       <c r="AC476" s="3"/>
       <c r="AD476" s="3"/>
     </row>
-    <row r="477" spans="1:30" ht="12.75" hidden="1">
+    <row r="477" spans="1:30" ht="12.75">
       <c r="A477" s="4">
         <v>31581370866</v>
       </c>
@@ -46077,7 +46077,7 @@
       <c r="AC477" s="3"/>
       <c r="AD477" s="3"/>
     </row>
-    <row r="478" spans="1:30" ht="12.75" hidden="1">
+    <row r="478" spans="1:30" ht="12.75">
       <c r="A478" s="4">
         <v>41281024616</v>
       </c>
@@ -46153,7 +46153,7 @@
       <c r="AC478" s="3"/>
       <c r="AD478" s="3"/>
     </row>
-    <row r="479" spans="1:30" ht="12.75" hidden="1">
+    <row r="479" spans="1:30" ht="12.75">
       <c r="A479" s="4">
         <v>31581011046</v>
       </c>
@@ -46229,7 +46229,7 @@
       <c r="AC479" s="3"/>
       <c r="AD479" s="3"/>
     </row>
-    <row r="480" spans="1:30" ht="12.75" hidden="1">
+    <row r="480" spans="1:30" ht="12.75">
       <c r="A480" s="4">
         <v>13081281806</v>
       </c>
@@ -46305,7 +46305,7 @@
       <c r="AC480" s="3"/>
       <c r="AD480" s="3"/>
     </row>
-    <row r="481" spans="1:30" ht="12.75" hidden="1">
+    <row r="481" spans="1:30" ht="12.75">
       <c r="A481" s="4">
         <v>51581197476</v>
       </c>
@@ -46381,7 +46381,7 @@
       <c r="AC481" s="3"/>
       <c r="AD481" s="3"/>
     </row>
-    <row r="482" spans="1:30" ht="12.75" hidden="1">
+    <row r="482" spans="1:30" ht="12.75">
       <c r="A482" s="4">
         <v>15288006726</v>
       </c>
@@ -46457,7 +46457,7 @@
       <c r="AC482" s="3"/>
       <c r="AD482" s="3"/>
     </row>
-    <row r="483" spans="1:30" ht="12.75" hidden="1">
+    <row r="483" spans="1:30" ht="12.75">
       <c r="A483" s="4">
         <v>22081193306</v>
       </c>
@@ -46533,7 +46533,7 @@
       <c r="AC483" s="3"/>
       <c r="AD483" s="3"/>
     </row>
-    <row r="484" spans="1:30" ht="12.75" hidden="1">
+    <row r="484" spans="1:30" ht="12.75">
       <c r="A484" s="4">
         <v>20681402546</v>
       </c>
@@ -46609,7 +46609,7 @@
       <c r="AC484" s="3"/>
       <c r="AD484" s="3"/>
     </row>
-    <row r="485" spans="1:30" ht="12.75" hidden="1">
+    <row r="485" spans="1:30" ht="12.75">
       <c r="A485" s="4">
         <v>12181248376</v>
       </c>
@@ -46685,7 +46685,7 @@
       <c r="AC485" s="3"/>
       <c r="AD485" s="3"/>
     </row>
-    <row r="486" spans="1:30" ht="12.75" hidden="1">
+    <row r="486" spans="1:30" ht="12.75">
       <c r="A486" s="4">
         <v>31381028066</v>
       </c>
@@ -46759,7 +46759,7 @@
       <c r="AC486" s="3"/>
       <c r="AD486" s="3"/>
     </row>
-    <row r="487" spans="1:30" ht="12.75" hidden="1">
+    <row r="487" spans="1:30" ht="12.75">
       <c r="A487" s="4">
         <v>91607733777</v>
       </c>
@@ -46835,7 +46835,7 @@
       <c r="AC487" s="3"/>
       <c r="AD487" s="3"/>
     </row>
-    <row r="488" spans="1:30" ht="12.75" hidden="1">
+    <row r="488" spans="1:30" ht="12.75">
       <c r="A488" s="4">
         <v>11481643366</v>
       </c>
@@ -46911,7 +46911,7 @@
       <c r="AC488" s="3"/>
       <c r="AD488" s="3"/>
     </row>
-    <row r="489" spans="1:30" ht="12.75" hidden="1">
+    <row r="489" spans="1:30" ht="12.75">
       <c r="A489" s="4">
         <v>31187000706</v>
       </c>
@@ -46987,7 +46987,7 @@
       <c r="AC489" s="3"/>
       <c r="AD489" s="3"/>
     </row>
-    <row r="490" spans="1:30" ht="12.75" hidden="1">
+    <row r="490" spans="1:30" ht="12.75">
       <c r="A490" s="4">
         <v>12281636436</v>
       </c>
@@ -47063,7 +47063,7 @@
       <c r="AC490" s="3"/>
       <c r="AD490" s="3"/>
     </row>
-    <row r="491" spans="1:30" ht="12.75" hidden="1">
+    <row r="491" spans="1:30" ht="12.75">
       <c r="A491" s="4">
         <v>13581793506</v>
       </c>
@@ -47137,7 +47137,7 @@
       <c r="AC491" s="3"/>
       <c r="AD491" s="3"/>
     </row>
-    <row r="492" spans="1:30" ht="12.75" hidden="1">
+    <row r="492" spans="1:30" ht="12.75">
       <c r="A492" s="4">
         <v>10181162936</v>
       </c>
@@ -47209,7 +47209,7 @@
       <c r="AC492" s="3"/>
       <c r="AD492" s="3"/>
     </row>
-    <row r="493" spans="1:30" ht="12.75" hidden="1">
+    <row r="493" spans="1:30" ht="12.75">
       <c r="A493" s="4">
         <v>11681055226</v>
       </c>
@@ -47285,7 +47285,7 @@
       <c r="AC493" s="3"/>
       <c r="AD493" s="3"/>
     </row>
-    <row r="494" spans="1:30" ht="12.75" hidden="1">
+    <row r="494" spans="1:30" ht="12.75">
       <c r="A494" s="4">
         <v>11481163776</v>
       </c>
@@ -47357,7 +47357,7 @@
       <c r="AC494" s="3"/>
       <c r="AD494" s="3"/>
     </row>
-    <row r="495" spans="1:30" ht="12.75" hidden="1">
+    <row r="495" spans="1:30" ht="12.75">
       <c r="A495" s="4">
         <v>40881003916</v>
       </c>
@@ -47433,7 +47433,7 @@
       <c r="AC495" s="3"/>
       <c r="AD495" s="3"/>
     </row>
-    <row r="496" spans="1:30" ht="12.75" hidden="1">
+    <row r="496" spans="1:30" ht="12.75">
       <c r="A496" s="4">
         <v>60681711466</v>
       </c>
@@ -47509,7 +47509,7 @@
       <c r="AC496" s="3"/>
       <c r="AD496" s="3"/>
     </row>
-    <row r="497" spans="1:30" ht="12.75" hidden="1">
+    <row r="497" spans="1:30" ht="12.75">
       <c r="A497" s="4">
         <v>11481163776</v>
       </c>
@@ -47585,7 +47585,7 @@
       <c r="AC497" s="3"/>
       <c r="AD497" s="3"/>
     </row>
-    <row r="498" spans="1:30" ht="12.75" hidden="1">
+    <row r="498" spans="1:30" ht="12.75">
       <c r="A498" s="4">
         <v>45486018886</v>
       </c>
@@ -47661,7 +47661,7 @@
       <c r="AC498" s="3"/>
       <c r="AD498" s="3"/>
     </row>
-    <row r="499" spans="1:30" ht="12.75" hidden="1">
+    <row r="499" spans="1:30" ht="12.75">
       <c r="A499" s="4">
         <v>17186024736</v>
       </c>
@@ -47737,7 +47737,7 @@
       <c r="AC499" s="3"/>
       <c r="AD499" s="3"/>
     </row>
-    <row r="500" spans="1:30" ht="12.75" hidden="1">
+    <row r="500" spans="1:30" ht="12.75">
       <c r="A500" s="4">
         <v>12681230946</v>
       </c>
@@ -47813,7 +47813,7 @@
       <c r="AC500" s="3"/>
       <c r="AD500" s="3"/>
     </row>
-    <row r="501" spans="1:30" ht="12.75" hidden="1">
+    <row r="501" spans="1:30" ht="12.75">
       <c r="A501" s="4">
         <v>13581019306</v>
       </c>
@@ -47893,7 +47893,7 @@
       <c r="AC501" s="3"/>
       <c r="AD501" s="3"/>
     </row>
-    <row r="502" spans="1:30" ht="12.75" hidden="1">
+    <row r="502" spans="1:30" ht="12.75">
       <c r="A502" s="4">
         <v>22081224606</v>
       </c>
@@ -47973,7 +47973,7 @@
       <c r="AC502" s="3"/>
       <c r="AD502" s="3"/>
     </row>
-    <row r="503" spans="1:30" ht="12.75" hidden="1">
+    <row r="503" spans="1:30" ht="12.75">
       <c r="A503" s="4">
         <v>20681402546</v>
       </c>
@@ -48053,7 +48053,7 @@
       <c r="AC503" s="3"/>
       <c r="AD503" s="3"/>
     </row>
-    <row r="504" spans="1:30" ht="12.75" hidden="1">
+    <row r="504" spans="1:30" ht="12.75">
       <c r="A504" s="4">
         <v>41681133686</v>
       </c>
@@ -48133,7 +48133,7 @@
       <c r="AC504" s="3"/>
       <c r="AD504" s="3"/>
     </row>
-    <row r="505" spans="1:30" ht="12.75" hidden="1">
+    <row r="505" spans="1:30" ht="12.75">
       <c r="A505" s="4">
         <v>40281215166</v>
       </c>
@@ -48213,7 +48213,7 @@
       <c r="AC505" s="3"/>
       <c r="AD505" s="3"/>
     </row>
-    <row r="506" spans="1:30" ht="12.75" hidden="1">
+    <row r="506" spans="1:30" ht="12.75">
       <c r="A506" s="4">
         <v>12181368196</v>
       </c>
@@ -48293,7 +48293,7 @@
       <c r="AC506" s="3"/>
       <c r="AD506" s="3"/>
     </row>
-    <row r="507" spans="1:30" ht="12.75" hidden="1">
+    <row r="507" spans="1:30" ht="12.75">
       <c r="A507" s="4">
         <v>21188792406</v>
       </c>
@@ -48373,7 +48373,7 @@
       <c r="AC507" s="3"/>
       <c r="AD507" s="3"/>
     </row>
-    <row r="508" spans="1:30" ht="12.75" hidden="1">
+    <row r="508" spans="1:30" ht="12.75">
       <c r="A508" s="4">
         <v>10586241126</v>
       </c>
@@ -48453,7 +48453,7 @@
       <c r="AC508" s="3"/>
       <c r="AD508" s="3"/>
     </row>
-    <row r="509" spans="1:30" ht="12.75" hidden="1">
+    <row r="509" spans="1:30" ht="12.75">
       <c r="A509" s="4">
         <v>12281282916</v>
       </c>
@@ -48533,7 +48533,7 @@
       <c r="AC509" s="3"/>
       <c r="AD509" s="3"/>
     </row>
-    <row r="510" spans="1:30" ht="12.75" hidden="1">
+    <row r="510" spans="1:30" ht="12.75">
       <c r="A510" s="4">
         <v>76381005706</v>
       </c>
@@ -48613,7 +48613,7 @@
       <c r="AC510" s="3"/>
       <c r="AD510" s="3"/>
     </row>
-    <row r="511" spans="1:30" ht="12.75" hidden="1">
+    <row r="511" spans="1:30" ht="12.75">
       <c r="A511" s="4">
         <v>10181162936</v>
       </c>
@@ -48693,7 +48693,7 @@
       <c r="AC511" s="3"/>
       <c r="AD511" s="3"/>
     </row>
-    <row r="512" spans="1:30" ht="12.75" hidden="1">
+    <row r="512" spans="1:30" ht="12.75">
       <c r="A512" s="4">
         <v>13881085346</v>
       </c>
@@ -48771,7 +48771,7 @@
       <c r="AC512" s="3"/>
       <c r="AD512" s="3"/>
     </row>
-    <row r="513" spans="1:30" ht="12.75" hidden="1">
+    <row r="513" spans="1:30" ht="12.75">
       <c r="A513" s="4">
         <v>21481699656</v>
       </c>
@@ -48849,7 +48849,7 @@
       <c r="AC513" s="3"/>
       <c r="AD513" s="3"/>
     </row>
-    <row r="514" spans="1:30" ht="12.75" hidden="1">
+    <row r="514" spans="1:30" ht="12.75">
       <c r="A514" s="4">
         <v>45486018886</v>
       </c>
@@ -48929,7 +48929,7 @@
       <c r="AC514" s="3"/>
       <c r="AD514" s="3"/>
     </row>
-    <row r="515" spans="1:30" ht="12.75" hidden="1">
+    <row r="515" spans="1:30" ht="12.75">
       <c r="A515" s="4">
         <v>10581745436</v>
       </c>
@@ -49005,7 +49005,7 @@
       <c r="AC515" s="3"/>
       <c r="AD515" s="3"/>
     </row>
-    <row r="516" spans="1:30" ht="12.75" hidden="1">
+    <row r="516" spans="1:30" ht="12.75">
       <c r="A516" s="4">
         <v>11681350076</v>
       </c>
@@ -49081,7 +49081,7 @@
       <c r="AC516" s="3"/>
       <c r="AD516" s="3"/>
     </row>
-    <row r="517" spans="1:30" ht="12.75" hidden="1">
+    <row r="517" spans="1:30" ht="12.75">
       <c r="A517" s="4">
         <v>11481163776</v>
       </c>
@@ -49157,7 +49157,7 @@
       <c r="AC517" s="3"/>
       <c r="AD517" s="3"/>
     </row>
-    <row r="518" spans="1:30" ht="12.75" hidden="1">
+    <row r="518" spans="1:30" ht="12.75">
       <c r="A518" s="4">
         <v>50581048686</v>
       </c>
@@ -49237,7 +49237,7 @@
       <c r="AC518" s="3"/>
       <c r="AD518" s="3"/>
     </row>
-    <row r="519" spans="1:30" ht="12.75" hidden="1">
+    <row r="519" spans="1:30" ht="12.75">
       <c r="A519" s="4">
         <v>60981046846</v>
       </c>
@@ -49317,7 +49317,7 @@
       <c r="AC519" s="3"/>
       <c r="AD519" s="3"/>
     </row>
-    <row r="520" spans="1:30" ht="12.75" hidden="1">
+    <row r="520" spans="1:30" ht="12.75">
       <c r="A520" s="4">
         <v>10481734066</v>
       </c>
@@ -49401,7 +49401,7 @@
       <c r="AC520" s="3"/>
       <c r="AD520" s="3"/>
     </row>
-    <row r="521" spans="1:30" ht="12.75" hidden="1">
+    <row r="521" spans="1:30" ht="12.75">
       <c r="A521" s="4">
         <v>11681350076</v>
       </c>
@@ -49481,7 +49481,7 @@
       <c r="AC521" s="3"/>
       <c r="AD521" s="3"/>
     </row>
-    <row r="522" spans="1:30" ht="12.75" hidden="1">
+    <row r="522" spans="1:30" ht="12.75">
       <c r="A522" s="4">
         <v>13881085346</v>
       </c>
@@ -49559,7 +49559,7 @@
       <c r="AC522" s="3"/>
       <c r="AD522" s="3"/>
     </row>
-    <row r="523" spans="1:30" ht="12.75" hidden="1">
+    <row r="523" spans="1:30" ht="12.75">
       <c r="A523" s="4">
         <v>45081001646</v>
       </c>
@@ -49639,7 +49639,7 @@
       <c r="AC523" s="3"/>
       <c r="AD523" s="3"/>
     </row>
-    <row r="524" spans="1:30" ht="12.75" hidden="1">
+    <row r="524" spans="1:30" ht="12.75">
       <c r="A524" s="4">
         <v>45081001646</v>
       </c>
@@ -49719,7 +49719,7 @@
       <c r="AC524" s="3"/>
       <c r="AD524" s="3"/>
     </row>
-    <row r="525" spans="1:30" ht="12.75" hidden="1">
+    <row r="525" spans="1:30" ht="12.75">
       <c r="A525" s="4">
         <v>21586047856</v>
       </c>
@@ -49864,13 +49864,7 @@
       <c r="AD527" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB525" xr:uid="{E824F881-A833-4EF0-B5A0-C2F40F99F353}">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="500000000000;800000000000"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AB525" xr:uid="{E824F881-A833-4EF0-B5A0-C2F40F99F353}"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>